<commit_message>
in all models change Cross references to Database references to replace an ambiguous name with a clear one
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_dry_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_dry_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1700" windowWidth="25600" windowHeight="15540" tabRatio="500" activeTab="6"/>
+    <workbookView xWindow="1120" yWindow="1700" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="2" activeTab="12"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -24,7 +24,7 @@
     <sheet name="Biomass reactions" sheetId="14" r:id="rId10"/>
     <sheet name="Parameters" sheetId="5" r:id="rId11"/>
     <sheet name="References" sheetId="6" r:id="rId12"/>
-    <sheet name="Cross references" sheetId="12" r:id="rId13"/>
+    <sheet name="Database references" sheetId="12" r:id="rId13"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$E$3</definedName>
@@ -34,7 +34,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$J$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Submodels!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="150001" concurrentCalc="0"/>
+  <calcPr calcId="150001" iterateDelta="1E-4" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
       <x14:workbookPr defaultImageDpi="32767"/>
@@ -1257,7 +1257,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>
@@ -1841,7 +1841,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
+    <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
       <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
migrated models to have compartment attributes in biomass reactions
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_dry_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_dry_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1700" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="2" activeTab="12"/>
+    <workbookView xWindow="1120" yWindow="1700" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="2" activeTab="9"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="225" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="131">
   <si>
     <t>ID</t>
   </si>
@@ -1062,20 +1062,21 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="15" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="23.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="16384" width="10.83203125" style="15"/>
+    <col min="3" max="3" width="23.1640625" style="15" customWidth="1"/>
+    <col min="4" max="16384" width="10.83203125" style="15"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="14" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="14" t="s">
         <v>36</v>
       </c>
@@ -1083,13 +1084,16 @@
         <v>1</v>
       </c>
       <c r="C1" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="D1" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="D1" s="14" t="s">
+      <c r="E1" s="14" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2" s="18" t="s">
         <v>118</v>
       </c>
@@ -1097,6 +1101,9 @@
         <v>126</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>127</v>
       </c>
     </row>
@@ -1257,7 +1264,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <sheetData>

</xml_diff>

<commit_message>
update model files to match new models in wc_lang 'Functions', 'Observables', 'Stop conditions'
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_dry_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_dry_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1700" windowWidth="25600" windowHeight="15540" tabRatio="500" firstSheet="2" activeTab="9"/>
+    <workbookView xWindow="1120" yWindow="1700" windowWidth="32800" windowHeight="16160" tabRatio="500" firstSheet="2" activeTab="15"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -25,6 +25,9 @@
     <sheet name="Parameters" sheetId="5" r:id="rId11"/>
     <sheet name="References" sheetId="6" r:id="rId12"/>
     <sheet name="Database references" sheetId="12" r:id="rId13"/>
+    <sheet name="Functions" sheetId="15" r:id="rId14"/>
+    <sheet name="Observables" sheetId="16" r:id="rId15"/>
+    <sheet name="Stop conditions" sheetId="17" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$E$3</definedName>
@@ -1064,7 +1067,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
+    <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1301,6 +1304,44 @@
       </c>
     </row>
   </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="N18" sqref="N18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
add headers for new models
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_dry_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_dry_model.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1120" yWindow="1700" windowWidth="32800" windowHeight="16160" tabRatio="500" firstSheet="2" activeTab="15"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21140" tabRatio="500" firstSheet="2" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="8" r:id="rId1"/>
@@ -18,22 +18,22 @@
     <sheet name="Compartments" sheetId="2" r:id="rId4"/>
     <sheet name="Species types" sheetId="3" r:id="rId5"/>
     <sheet name="Concentrations" sheetId="10" r:id="rId6"/>
-    <sheet name="Reactions" sheetId="4" r:id="rId7"/>
-    <sheet name="Rate laws" sheetId="11" r:id="rId8"/>
-    <sheet name="Biomass components" sheetId="13" r:id="rId9"/>
-    <sheet name="Biomass reactions" sheetId="14" r:id="rId10"/>
-    <sheet name="Parameters" sheetId="5" r:id="rId11"/>
-    <sheet name="References" sheetId="6" r:id="rId12"/>
-    <sheet name="Database references" sheetId="12" r:id="rId13"/>
-    <sheet name="Functions" sheetId="15" r:id="rId14"/>
-    <sheet name="Observables" sheetId="16" r:id="rId15"/>
-    <sheet name="Stop conditions" sheetId="17" r:id="rId16"/>
+    <sheet name="Observables" sheetId="16" r:id="rId7"/>
+    <sheet name="Functions" sheetId="15" r:id="rId8"/>
+    <sheet name="Reactions" sheetId="4" r:id="rId9"/>
+    <sheet name="Rate laws" sheetId="11" r:id="rId10"/>
+    <sheet name="Biomass components" sheetId="13" r:id="rId11"/>
+    <sheet name="Biomass reactions" sheetId="14" r:id="rId12"/>
+    <sheet name="Parameters" sheetId="5" r:id="rId13"/>
+    <sheet name="Stop conditions" sheetId="17" r:id="rId14"/>
+    <sheet name="References" sheetId="6" r:id="rId15"/>
+    <sheet name="Database references" sheetId="12" r:id="rId16"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Compartments!$A$1:$E$3</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">Parameters!$A$1:$F$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">Reactions!$A$1:$D$5</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="11" hidden="1">References!$A$1:$E$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="12" hidden="1">Parameters!$A$1:$F$1</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="8" hidden="1">Reactions!$A$1:$D$5</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="14" hidden="1">References!$A$1:$E$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">'Species types'!$A$1:$J$6</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="2" hidden="1">Submodels!#REF!</definedName>
   </definedNames>
@@ -50,7 +50,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="227" uniqueCount="131">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="133">
   <si>
     <t>ID</t>
   </si>
@@ -443,6 +443,12 @@
   </si>
   <si>
     <t>Max flux</t>
+  </si>
+  <si>
+    <t>Observables</t>
+  </si>
+  <si>
+    <t>Expression</t>
   </si>
 </sst>
 </file>
@@ -1065,6 +1071,244 @@
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G6"/>
+  <sheetViews>
+    <sheetView zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1:H1048576"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="3" max="3" width="37.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="C1" s="5" t="s">
+        <v>50</v>
+      </c>
+      <c r="D1" s="5" t="s">
+        <v>51</v>
+      </c>
+      <c r="E1" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="F1" s="5" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="5" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C2" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="6">
+        <v>2000</v>
+      </c>
+      <c r="E3" s="1"/>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B4" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C4" t="s">
+        <v>104</v>
+      </c>
+      <c r="D4" s="6">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E4" s="6">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>98</v>
+      </c>
+      <c r="C5" t="s">
+        <v>100</v>
+      </c>
+      <c r="D5" s="6">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E5" s="6">
+        <v>1E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="C6" t="s">
+        <v>46</v>
+      </c>
+      <c r="D6" s="6">
+        <v>2.9999999999999997E-4</v>
+      </c>
+      <c r="E6" s="6">
+        <v>1E-3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:G5"/>
+  <sheetViews>
+    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
+      <selection activeCell="F8" sqref="F8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="13.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17" style="15" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.33203125" style="15" customWidth="1"/>
+    <col min="4" max="4" width="9.33203125" style="15" customWidth="1"/>
+    <col min="5" max="5" width="10.5" style="15" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" style="15" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.1640625" style="15" bestFit="1" customWidth="1"/>
+    <col min="8" max="16384" width="10.83203125" style="15"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="14" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="E1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>3</v>
+      </c>
+      <c r="G1" s="14" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A2" s="15" t="s">
+        <v>116</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>117</v>
+      </c>
+      <c r="C2" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D2" s="17">
+        <v>-3</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="G2" s="16"/>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A3" s="15" t="s">
+        <v>120</v>
+      </c>
+      <c r="B3" s="15" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D3" s="17">
+        <v>-4</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A4" s="15" t="s">
+        <v>122</v>
+      </c>
+      <c r="B4" s="15" t="s">
+        <v>123</v>
+      </c>
+      <c r="C4" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D4" s="17">
+        <v>1</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A5" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="15" t="s">
+        <v>125</v>
+      </c>
+      <c r="C5" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="D5" s="17">
+        <v>2</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="140" workbookViewId="0">
@@ -1115,7 +1359,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H2"/>
   <sheetViews>
@@ -1186,7 +1430,39 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:R1"/>
   <sheetViews>
@@ -1263,7 +1539,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J1"/>
   <sheetViews>
@@ -1304,44 +1580,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N18" sqref="N18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1887,6 +2125,73 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:F1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:F1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>45</v>
+      </c>
+      <c r="E1" t="s">
+        <v>131</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:E1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:E1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>37</v>
+      </c>
+      <c r="D1" t="s">
+        <v>132</v>
+      </c>
+      <c r="E1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:I5"/>
   <sheetViews>
     <sheetView zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="120" workbookViewId="0">
@@ -2028,242 +2333,4 @@
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
-  <sheetViews>
-    <sheetView zoomScale="161" zoomScaleNormal="161" zoomScalePageLayoutView="161" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1:H1048576"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="3" max="3" width="37.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
-        <v>48</v>
-      </c>
-      <c r="B1" s="5" t="s">
-        <v>49</v>
-      </c>
-      <c r="C1" s="5" t="s">
-        <v>50</v>
-      </c>
-      <c r="D1" s="5" t="s">
-        <v>51</v>
-      </c>
-      <c r="E1" s="5" t="s">
-        <v>52</v>
-      </c>
-      <c r="F1" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="5" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C2" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C3" t="s">
-        <v>99</v>
-      </c>
-      <c r="D3" s="6">
-        <v>2000</v>
-      </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B4" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C4" t="s">
-        <v>104</v>
-      </c>
-      <c r="D4" s="6">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="E4" s="6">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="B5" s="7" t="s">
-        <v>98</v>
-      </c>
-      <c r="C5" t="s">
-        <v>100</v>
-      </c>
-      <c r="D5" s="6">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="E5" s="6">
-        <v>1E-3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A6" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="B6" s="7" t="s">
-        <v>86</v>
-      </c>
-      <c r="C6" t="s">
-        <v>46</v>
-      </c>
-      <c r="D6" s="6">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="E6" s="6">
-        <v>1E-3</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G5"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" zoomScalePageLayoutView="130" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="13.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="17" style="15" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.33203125" style="15" customWidth="1"/>
-    <col min="4" max="4" width="9.33203125" style="15" customWidth="1"/>
-    <col min="5" max="5" width="10.5" style="15" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="9.33203125" style="15" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.1640625" style="15" bestFit="1" customWidth="1"/>
-    <col min="8" max="16384" width="10.83203125" style="15"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A1" s="14" t="s">
-        <v>36</v>
-      </c>
-      <c r="B1" s="14" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D1" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="E1" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="14" t="s">
-        <v>3</v>
-      </c>
-      <c r="G1" s="14" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A2" s="15" t="s">
-        <v>116</v>
-      </c>
-      <c r="B2" s="15" t="s">
-        <v>117</v>
-      </c>
-      <c r="C2" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D2" s="17">
-        <v>-3</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="F2" s="16" t="s">
-        <v>119</v>
-      </c>
-      <c r="G2" s="16"/>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="15" t="s">
-        <v>120</v>
-      </c>
-      <c r="B3" s="15" t="s">
-        <v>121</v>
-      </c>
-      <c r="C3" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D3" s="17">
-        <v>-4</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A4" s="15" t="s">
-        <v>122</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>123</v>
-      </c>
-      <c r="C4" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D4" s="17">
-        <v>1</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="15" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="15" t="s">
-        <v>125</v>
-      </c>
-      <c r="C5" s="16" t="s">
-        <v>118</v>
-      </c>
-      <c r="D5" s="17">
-        <v>2</v>
-      </c>
-      <c r="E5" t="s">
-        <v>34</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
implement sampling of initial species counts
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_dry_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_dry_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="993" activeTab="9"/>
+    <workbookView windowWidth="19800" windowHeight="6840" tabRatio="993" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Model" sheetId="1" r:id="rId1"/>
@@ -668,12 +668,12 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="176" formatCode="0.000E+00"/>
+    <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="176" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
     <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
-    <numFmt numFmtId="177" formatCode="0.000E+00"/>
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="24">
     <font>
@@ -702,17 +702,17 @@
       <charset val="1"/>
     </font>
     <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="10"/>
       <name val="Arial"/>
       <charset val="134"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF800080"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -731,7 +731,23 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF800080"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -745,18 +761,10 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -768,8 +776,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -777,9 +793,16 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="3"/>
+      <color rgb="FF3F3F3F"/>
       <name val="Calibri"/>
-      <charset val="134"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -799,25 +822,16 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
+      <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -828,23 +842,9 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color rgb="FF0000FF"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -865,12 +865,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -883,7 +877,97 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor rgb="FFF2F2F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -895,37 +979,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFC7CE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -943,13 +997,37 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
+        <fgColor theme="9" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -961,91 +1039,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFCC99"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFC6EFCE"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1098,21 +1098,6 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left/>
       <right/>
       <top/>
@@ -1124,11 +1109,9 @@
     <border>
       <left/>
       <right/>
-      <top style="thin">
-        <color theme="4"/>
-      </top>
-      <bottom style="double">
-        <color theme="4"/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1148,6 +1131,21 @@
       <diagonal/>
     </border>
     <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left/>
       <right/>
       <top/>
@@ -1159,145 +1157,147 @@
     <border>
       <left/>
       <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
+      <top style="thin">
+        <color theme="4"/>
+      </top>
+      <bottom style="double">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="6" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="17" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="23" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="7" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="7" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="12" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="17" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="5" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="4" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="23" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="5" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1349,17 +1349,17 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="35" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="35" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="177" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1893,7 +1893,7 @@
   <sheetPr/>
   <dimension ref="A1:M5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -3119,18 +3119,20 @@
   <sheetPr/>
   <dimension ref="A1:AMO3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="H1" sqref="H1:L1"/>
+      <selection pane="bottomRight" activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2"/>
   <cols>
     <col min="1" max="8" width="8.78333333333333" style="13"/>
-    <col min="9" max="1030" width="8.78333333333333" style="20"/>
+    <col min="9" max="9" width="8.78333333333333" style="20"/>
+    <col min="10" max="10" width="9.375" style="20"/>
+    <col min="11" max="1030" width="8.78333333333333" style="20"/>
     <col min="1031" max="16384" width="9" style="20"/>
   </cols>
   <sheetData>
@@ -3249,11 +3251,11 @@
       <c r="H3" s="2" t="s">
         <v>54</v>
       </c>
-      <c r="I3" s="2">
-        <v>1</v>
-      </c>
-      <c r="J3" s="2">
-        <v>0</v>
+      <c r="I3" s="6">
+        <v>1e-12</v>
+      </c>
+      <c r="J3" s="6">
+        <v>1e-13</v>
       </c>
       <c r="K3" s="2" t="s">
         <v>55</v>

</xml_diff>

<commit_message>
updating for adding structure to wc_lang
</commit_message>
<xml_diff>
--- a/tests/multialgorithm/fixtures/test_dry_model.xlsx
+++ b/tests/multialgorithm/fixtures/test_dry_model.xlsx
@@ -5,7 +5,7 @@
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
-    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" firstSheet="9" activeTab="19"/>
+    <workbookView windowWidth="28695" windowHeight="14070" tabRatio="993" activeTab="13"/>
   </bookViews>
   <sheets>
     <sheet name="Table of contents" sheetId="25" r:id="rId1"/>
@@ -61,7 +61,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="538" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="243">
   <si>
     <t>Table</t>
   </si>
@@ -282,9 +282,6 @@
     <t>Initial density</t>
   </si>
   <si>
-    <t>Value</t>
-  </si>
-  <si>
     <t>c</t>
   </si>
   <si>
@@ -474,7 +471,7 @@
     <t>e / density_c</t>
   </si>
   <si>
-    <t>Flux</t>
+    <t>Flux bounds</t>
   </si>
   <si>
     <t>Submodel</t>
@@ -601,6 +598,9 @@
   </si>
   <si>
     <t>dFBA objective reaction</t>
+  </si>
+  <si>
+    <t>Value</t>
   </si>
   <si>
     <t>dfba-net-species-Metabolism_biomass-specie_1[c]</t>
@@ -797,11 +797,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="6">
+    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="176" formatCode="0.000E+00"/>
-    <numFmt numFmtId="41" formatCode="_(* #,##0_);_(* \(#,##0\);_(* &quot;-&quot;_);_(@_)"/>
+    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="177" formatCode="&quot;TRUE&quot;;&quot;TRUE&quot;;&quot;FALSE&quot;"/>
-    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="42" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="26">
@@ -851,22 +851,8 @@
       <charset val="134"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <charset val="134"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFFFFFF"/>
+      <color theme="0"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -879,48 +865,9 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="18"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
+      <sz val="10"/>
+      <name val="Arial"/>
       <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
-      <name val="Calibri"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
     </font>
     <font>
       <b/>
@@ -933,6 +880,21 @@
     <font>
       <b/>
       <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
       <color theme="3"/>
       <name val="Calibri"/>
       <charset val="134"/>
@@ -947,16 +909,32 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
+      <u/>
       <sz val="11"/>
-      <color rgb="FF3F3F3F"/>
+      <color rgb="FF800080"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FF9C0006"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFFFFFF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -977,9 +955,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF800080"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -987,6 +964,29 @@
     <font>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FF3F3F3F"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="Calibri"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -1013,7 +1013,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFA5A5A5"/>
+        <fgColor theme="6" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1025,13 +1037,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1043,7 +1049,67 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFA5A5A5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1055,13 +1121,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFFFCC"/>
+        <fgColor theme="7" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="5" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1073,13 +1145,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor rgb="FFFFFFCC"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1091,91 +1181,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="8" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1187,13 +1193,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.799981688894314"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1216,17 +1216,11 @@
       <diagonal/>
     </border>
     <border>
-      <left style="double">
-        <color rgb="FF3F3F3F"/>
-      </left>
-      <right style="double">
-        <color rgb="FF3F3F3F"/>
-      </right>
-      <top style="double">
-        <color rgb="FF3F3F3F"/>
-      </top>
-      <bottom style="double">
-        <color rgb="FF3F3F3F"/>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
       </bottom>
       <diagonal/>
     </border>
@@ -1246,40 +1240,16 @@
       <diagonal/>
     </border>
     <border>
-      <left style="thin">
-        <color rgb="FFB2B2B2"/>
-      </left>
-      <right style="thin">
-        <color rgb="FFB2B2B2"/>
-      </right>
-      <top style="thin">
-        <color rgb="FFB2B2B2"/>
-      </top>
-      <bottom style="thin">
-        <color rgb="FFB2B2B2"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="thin">
+      <left style="double">
         <color rgb="FF3F3F3F"/>
       </left>
-      <right style="thin">
+      <right style="double">
         <color rgb="FF3F3F3F"/>
       </right>
-      <top style="thin">
+      <top style="double">
         <color rgb="FF3F3F3F"/>
       </top>
-      <bottom style="thin">
+      <bottom style="double">
         <color rgb="FF3F3F3F"/>
       </bottom>
       <diagonal/>
@@ -1313,139 +1283,169 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFB2B2B2"/>
+      </left>
+      <right style="thin">
+        <color rgb="FFB2B2B2"/>
+      </right>
+      <top style="thin">
+        <color rgb="FFB2B2B2"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color rgb="FF3F3F3F"/>
+      </left>
+      <right style="thin">
+        <color rgb="FF3F3F3F"/>
+      </right>
+      <top style="thin">
+        <color rgb="FF3F3F3F"/>
+      </top>
+      <bottom style="thin">
+        <color rgb="FF3F3F3F"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="12" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="12" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="12" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="23" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="7" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="44" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="11" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="24" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="10" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="7" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="23" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="44" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="26" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="21" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="6" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="41" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="41" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="42" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="42" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="4" borderId="2" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="43" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="9" fontId="8" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="9" fontId="9" fillId="0" borderId="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
@@ -1494,9 +1494,6 @@
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -1527,6 +1524,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="35" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -2216,7 +2216,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="5" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="5" t="s">
         <v>71</v>
@@ -2273,7 +2273,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>71</v>
@@ -2296,24 +2296,24 @@
     </row>
     <row r="2" customHeight="1" spans="1:4">
       <c r="A2" s="1" t="s">
+        <v>132</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>134</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:4">
       <c r="A3" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="C3" s="1" t="s">
         <v>135</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>136</v>
-      </c>
       <c r="D3" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
   </sheetData>
@@ -2333,7 +2333,7 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="L4" sqref="L4"/>
+      <selection pane="bottomRight" activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="5"/>
@@ -2346,22 +2346,22 @@
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:14">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="20" t="s">
-        <v>137</v>
-      </c>
-      <c r="H1" s="20"/>
-      <c r="I1" s="20"/>
-      <c r="J1" s="18"/>
-      <c r="K1" s="18"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="18"/>
-      <c r="N1" s="18"/>
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="19" t="s">
+        <v>136</v>
+      </c>
+      <c r="H1" s="19"/>
+      <c r="I1" s="19"/>
+      <c r="J1" s="17"/>
+      <c r="K1" s="17"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="17"/>
+      <c r="N1" s="17"/>
     </row>
     <row r="2" s="3" customFormat="1" customHeight="1" spans="1:14">
       <c r="A2" s="2" t="s">
@@ -2371,22 +2371,22 @@
         <v>27</v>
       </c>
       <c r="C2" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D2" s="2" t="s">
         <v>138</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="E2" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="F2" s="2" t="s">
         <v>140</v>
       </c>
-      <c r="F2" s="2" t="s">
+      <c r="G2" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="H2" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="H2" s="2" t="s">
-        <v>143</v>
       </c>
       <c r="I2" s="2" t="s">
         <v>71</v>
@@ -2409,105 +2409,105 @@
     </row>
     <row r="3" customHeight="1" spans="1:10">
       <c r="A3" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>144</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>145</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D3" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="E3" s="20">
+        <v>0</v>
+      </c>
+      <c r="F3" s="20" t="s">
         <v>146</v>
       </c>
-      <c r="E3" s="21">
+      <c r="G3" s="20">
         <v>0</v>
       </c>
-      <c r="F3" s="21" t="s">
+      <c r="H3" s="20">
+        <v>1</v>
+      </c>
+      <c r="I3" s="21" t="s">
         <v>147</v>
       </c>
-      <c r="G3" s="21">
-        <v>0</v>
-      </c>
-      <c r="H3" s="21">
-        <v>1</v>
-      </c>
-      <c r="I3" s="22" t="s">
-        <v>148</v>
-      </c>
-      <c r="J3" s="23"/>
+      <c r="J3" s="22"/>
     </row>
     <row r="4" customHeight="1" spans="1:10">
       <c r="A4" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="B4" s="1" t="s">
         <v>149</v>
-      </c>
-      <c r="B4" s="1" t="s">
-        <v>150</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="E4" s="21">
+        <v>150</v>
+      </c>
+      <c r="E4" s="20">
         <v>1</v>
       </c>
-      <c r="F4" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G4" s="21"/>
-      <c r="H4" s="21"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="23"/>
+      <c r="F4" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G4" s="20"/>
+      <c r="H4" s="20"/>
+      <c r="I4" s="21"/>
+      <c r="J4" s="22"/>
     </row>
     <row r="5" customHeight="1" spans="1:10">
       <c r="A5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B5" s="1" t="s">
         <v>152</v>
-      </c>
-      <c r="B5" s="1" t="s">
-        <v>153</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>58</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>154</v>
-      </c>
-      <c r="E5" s="21">
+        <v>153</v>
+      </c>
+      <c r="E5" s="20">
         <v>1</v>
       </c>
-      <c r="F5" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
+      <c r="F5" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G5" s="21"/>
+      <c r="H5" s="21"/>
+      <c r="I5" s="21"/>
+      <c r="J5" s="21"/>
     </row>
     <row r="6" customHeight="1" spans="1:10">
       <c r="A6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="B6" s="1" t="s">
         <v>155</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>156</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>58</v>
       </c>
-      <c r="D6" s="19" t="s">
-        <v>157</v>
-      </c>
-      <c r="E6" s="21">
+      <c r="D6" s="18" t="s">
+        <v>156</v>
+      </c>
+      <c r="E6" s="20">
         <v>0</v>
       </c>
-      <c r="F6" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
+      <c r="F6" s="20" t="s">
+        <v>146</v>
+      </c>
+      <c r="G6" s="21"/>
+      <c r="H6" s="21"/>
+      <c r="I6" s="21"/>
+      <c r="J6" s="21"/>
     </row>
   </sheetData>
   <autoFilter ref="A2:D6">
@@ -2557,16 +2557,16 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>158</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>159</v>
-      </c>
       <c r="E1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="G1" s="2" t="s">
         <v>71</v>
@@ -2589,19 +2589,19 @@
     </row>
     <row r="2" customHeight="1" spans="1:11">
       <c r="A2" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>160</v>
       </c>
-      <c r="C2" s="1" t="s">
-        <v>144</v>
-      </c>
-      <c r="D2" s="10" t="s">
+      <c r="F2" s="1" t="s">
         <v>161</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>162</v>
-      </c>
       <c r="G2" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H2"/>
       <c r="I2"/>
@@ -2610,19 +2610,19 @@
     </row>
     <row r="3" customHeight="1" spans="1:11">
       <c r="A3" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>148</v>
+      </c>
+      <c r="D3" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F3" s="1" t="s">
         <v>163</v>
       </c>
-      <c r="C3" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>164</v>
-      </c>
       <c r="G3" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H3"/>
       <c r="I3"/>
@@ -2631,19 +2631,19 @@
     </row>
     <row r="4" customHeight="1" spans="1:11">
       <c r="A4" s="1" t="s">
+        <v>164</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D4" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F4" s="1" t="s">
         <v>165</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D4" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="F4" s="1" t="s">
-        <v>166</v>
-      </c>
       <c r="G4" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H4"/>
       <c r="I4"/>
@@ -2652,19 +2652,19 @@
     </row>
     <row r="5" customHeight="1" spans="1:13">
       <c r="A5" s="1" t="s">
+        <v>166</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="D5" s="10" t="s">
         <v>167</v>
       </c>
-      <c r="C5" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="D5" s="10" t="s">
+      <c r="F5" s="1" t="s">
         <v>168</v>
       </c>
-      <c r="F5" s="1" t="s">
-        <v>169</v>
-      </c>
       <c r="G5" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H5"/>
       <c r="I5"/>
@@ -2674,19 +2674,19 @@
     </row>
     <row r="6" customHeight="1" spans="1:13">
       <c r="A6" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>154</v>
+      </c>
+      <c r="D6" s="10" t="s">
+        <v>160</v>
+      </c>
+      <c r="F6" s="1" t="s">
         <v>170</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>155</v>
-      </c>
-      <c r="D6" s="10" t="s">
-        <v>161</v>
-      </c>
-      <c r="F6" s="1" t="s">
-        <v>171</v>
-      </c>
       <c r="G6" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="H6"/>
       <c r="I6"/>
@@ -2710,100 +2710,81 @@
 <file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:L3"/>
+  <dimension ref="A1:L2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="E6" sqref="E6"/>
+      <selection pane="bottomRight" activeCell="L10" sqref="L10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="1"/>
   <cols>
     <col min="1" max="16384" width="9" style="15"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:12">
-      <c r="A1" s="1"/>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="16" t="s">
-        <v>132</v>
-      </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="1"/>
-      <c r="G1" s="1"/>
-      <c r="H1" s="1"/>
-      <c r="I1" s="1"/>
-      <c r="J1" s="1"/>
-      <c r="K1" s="1"/>
-      <c r="L1" s="1"/>
+      <c r="A1" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>172</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="K1" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="L1" s="2" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="2" customHeight="1" spans="1:12">
-      <c r="A2" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>138</v>
-      </c>
-      <c r="D2" s="2" t="s">
-        <v>73</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>71</v>
-      </c>
-      <c r="F2" s="2" t="s">
-        <v>172</v>
-      </c>
-      <c r="G2" s="2" t="s">
+    <row r="2" customHeight="1" spans="1:7">
+      <c r="A2" s="1" t="s">
         <v>173</v>
       </c>
-      <c r="H2" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="J2" s="2" t="s">
-        <v>21</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>41</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="3" customHeight="1" spans="1:7">
-      <c r="A3" s="1" t="s">
+      <c r="B2" s="1"/>
+      <c r="C2" s="16" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" s="10" t="s">
         <v>174</v>
       </c>
-      <c r="B3" s="1"/>
-      <c r="C3" s="17" t="s">
-        <v>54</v>
-      </c>
-      <c r="D3" s="10" t="s">
-        <v>175</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="G3" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>39</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="D1:E1"/>
-  </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
@@ -2837,13 +2818,13 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>71</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="F1" s="2" t="s">
         <v>40</v>
@@ -2863,22 +2844,22 @@
     </row>
     <row r="2" customHeight="1" spans="1:9">
       <c r="A2" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B2" s="10" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>54</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="I2" s="10" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
   </sheetData>
@@ -2916,13 +2897,13 @@
         <v>27</v>
       </c>
       <c r="C1" s="13" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="D1" s="13" t="s">
         <v>9</v>
       </c>
       <c r="E1" s="13" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
       <c r="F1" s="13" t="s">
         <v>71</v>
@@ -2951,16 +2932,16 @@
         <v>181</v>
       </c>
       <c r="C2" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="E2" s="14">
         <v>-3</v>
       </c>
       <c r="F2" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="J2" s="10" t="s">
         <v>182</v>
@@ -2974,16 +2955,16 @@
         <v>184</v>
       </c>
       <c r="C3" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E3" s="14">
         <v>-4</v>
       </c>
       <c r="F3" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:6">
@@ -2994,16 +2975,16 @@
         <v>186</v>
       </c>
       <c r="C4" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E4" s="14">
         <v>1</v>
       </c>
       <c r="F4" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:6">
@@ -3014,16 +2995,16 @@
         <v>188</v>
       </c>
       <c r="C5" s="10" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="E5" s="14">
         <v>2</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
   </sheetData>
@@ -3063,10 +3044,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>189</v>
@@ -3101,7 +3082,7 @@
         <v>0</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="J2" s="1" t="s">
         <v>192</v>
@@ -3146,7 +3127,7 @@
         <v>0.0003</v>
       </c>
       <c r="F5" s="9" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:6">
@@ -3188,12 +3169,12 @@
         <v>0.001</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:6">
       <c r="A9" s="1" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D9" s="1">
         <v>1100</v>
@@ -3204,7 +3185,7 @@
     </row>
     <row r="10" customHeight="1" spans="1:6">
       <c r="A10" s="1" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="D10" s="1">
         <v>1000</v>
@@ -3261,7 +3242,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>71</v>
@@ -3337,7 +3318,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>189</v>
@@ -3346,7 +3327,7 @@
         <v>71</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>4</v>
@@ -3535,7 +3516,7 @@
   <sheetPr/>
   <dimension ref="A1:M10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection/>
       <selection pane="topRight"/>
@@ -3565,7 +3546,7 @@
         <v>27</v>
       </c>
       <c r="C2" s="5" t="s">
-        <v>73</v>
+        <v>179</v>
       </c>
       <c r="D2" s="5" t="s">
         <v>189</v>
@@ -3574,7 +3555,7 @@
         <v>71</v>
       </c>
       <c r="F2" s="5" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G2" s="5" t="s">
         <v>27</v>
@@ -3683,7 +3664,7 @@
         <v>218</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>219</v>
@@ -3818,7 +3799,7 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>235</v>
@@ -4019,12 +4000,12 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="13.5" outlineLevelRow="2"/>
   <cols>
-    <col min="1" max="7" width="8.78333333333333" style="17"/>
-    <col min="8" max="1026" width="8.78333333333333" style="25"/>
-    <col min="1027" max="16384" width="9" style="25"/>
+    <col min="1" max="7" width="8.78333333333333" style="16"/>
+    <col min="8" max="1026" width="8.78333333333333" style="24"/>
+    <col min="1027" max="16384" width="9" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" s="18" customFormat="1" ht="15" customHeight="1" spans="1:1025">
+    <row r="1" s="17" customFormat="1" ht="15" customHeight="1" spans="1:1025">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -4049,30 +4030,30 @@
       <c r="H1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AMI1" s="25"/>
-      <c r="AMJ1" s="25"/>
-      <c r="AMK1" s="25"/>
+      <c r="AMI1" s="24"/>
+      <c r="AMJ1" s="24"/>
+      <c r="AMK1" s="24"/>
     </row>
     <row r="2" ht="15" customHeight="1" spans="1:7">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
         <v>54</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="B2" s="16" t="s">
         <v>55</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>56</v>
       </c>
       <c r="D2" s="28"/>
-      <c r="G2" s="17" t="s">
+      <c r="G2" s="16" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="3" ht="15" customHeight="1" spans="1:3">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
         <v>58</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="B3" s="16" t="s">
         <v>59</v>
       </c>
       <c r="C3" s="1" t="s">
@@ -4096,1055 +4077,1055 @@
       <selection/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="A1" sqref="$A1:$XFD2"/>
+      <selection pane="bottomRight" activeCell="M1" sqref="M1:P4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1" outlineLevelRow="3"/>
   <cols>
-    <col min="1" max="8" width="8.78333333333333" style="17"/>
-    <col min="9" max="9" width="8.78333333333333" style="25"/>
-    <col min="10" max="10" width="9.375" style="25"/>
-    <col min="11" max="1033" width="8.78333333333333" style="25"/>
-    <col min="1034" max="16384" width="9" style="25"/>
+    <col min="1" max="8" width="8.78333333333333" style="16"/>
+    <col min="9" max="9" width="8.78333333333333" style="24"/>
+    <col min="10" max="10" width="9.375" style="24"/>
+    <col min="11" max="1035" width="8.78333333333333" style="24"/>
+    <col min="1036" max="16384" width="9" style="24"/>
   </cols>
   <sheetData>
     <row r="1" customHeight="1" spans="1:16384">
-      <c r="A1" s="18"/>
-      <c r="B1" s="18"/>
-      <c r="C1" s="18"/>
-      <c r="D1" s="18"/>
-      <c r="E1" s="18"/>
-      <c r="F1" s="18"/>
-      <c r="G1" s="18"/>
-      <c r="H1" s="16" t="s">
+      <c r="A1" s="17"/>
+      <c r="B1" s="17"/>
+      <c r="C1" s="17"/>
+      <c r="D1" s="17"/>
+      <c r="E1" s="17"/>
+      <c r="F1" s="17"/>
+      <c r="G1" s="17"/>
+      <c r="H1" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="I1" s="16"/>
-      <c r="J1" s="16"/>
-      <c r="K1" s="16"/>
-      <c r="L1" s="18"/>
-      <c r="M1" s="16" t="s">
+      <c r="I1" s="27"/>
+      <c r="J1" s="27"/>
+      <c r="K1" s="27"/>
+      <c r="L1" s="17"/>
+      <c r="M1" s="27" t="s">
         <v>62</v>
       </c>
-      <c r="N1" s="16"/>
-      <c r="O1" s="18"/>
-      <c r="P1" s="18"/>
-      <c r="Q1" s="18"/>
-      <c r="R1" s="18"/>
-      <c r="S1" s="18"/>
-      <c r="T1" s="18"/>
-      <c r="U1" s="18"/>
-      <c r="V1" s="18"/>
-      <c r="W1" s="18"/>
-      <c r="X1" s="18"/>
-      <c r="Y1" s="18"/>
-      <c r="Z1" s="18"/>
-      <c r="AA1" s="18"/>
-      <c r="AB1" s="18"/>
-      <c r="AC1" s="18"/>
-      <c r="AD1" s="18"/>
-      <c r="AE1" s="18"/>
-      <c r="AF1" s="18"/>
-      <c r="AG1" s="18"/>
-      <c r="AH1" s="18"/>
-      <c r="AI1" s="18"/>
-      <c r="AJ1" s="18"/>
-      <c r="AK1" s="18"/>
-      <c r="AL1" s="18"/>
-      <c r="AM1" s="18"/>
-      <c r="AN1" s="18"/>
-      <c r="AO1" s="18"/>
-      <c r="AP1" s="18"/>
-      <c r="AQ1" s="18"/>
-      <c r="AR1" s="18"/>
-      <c r="AS1" s="18"/>
-      <c r="AT1" s="18"/>
-      <c r="AU1" s="18"/>
-      <c r="AV1" s="18"/>
-      <c r="AW1" s="18"/>
-      <c r="AX1" s="18"/>
-      <c r="AY1" s="18"/>
-      <c r="AZ1" s="18"/>
-      <c r="BA1" s="18"/>
-      <c r="BB1" s="18"/>
-      <c r="BC1" s="18"/>
-      <c r="BD1" s="18"/>
-      <c r="BE1" s="18"/>
-      <c r="BF1" s="18"/>
-      <c r="BG1" s="18"/>
-      <c r="BH1" s="18"/>
-      <c r="BI1" s="18"/>
-      <c r="BJ1" s="18"/>
-      <c r="BK1" s="18"/>
-      <c r="BL1" s="18"/>
-      <c r="BM1" s="18"/>
-      <c r="BN1" s="18"/>
-      <c r="BO1" s="18"/>
-      <c r="BP1" s="18"/>
-      <c r="BQ1" s="18"/>
-      <c r="BR1" s="18"/>
-      <c r="BS1" s="18"/>
-      <c r="BT1" s="18"/>
-      <c r="BU1" s="18"/>
-      <c r="BV1" s="18"/>
-      <c r="BW1" s="18"/>
-      <c r="BX1" s="18"/>
-      <c r="BY1" s="18"/>
-      <c r="BZ1" s="18"/>
-      <c r="CA1" s="18"/>
-      <c r="CB1" s="18"/>
-      <c r="CC1" s="18"/>
-      <c r="CD1" s="18"/>
-      <c r="CE1" s="18"/>
-      <c r="CF1" s="18"/>
-      <c r="CG1" s="18"/>
-      <c r="CH1" s="18"/>
-      <c r="CI1" s="18"/>
-      <c r="CJ1" s="18"/>
-      <c r="CK1" s="18"/>
-      <c r="CL1" s="18"/>
-      <c r="CM1" s="18"/>
-      <c r="CN1" s="18"/>
-      <c r="CO1" s="18"/>
-      <c r="CP1" s="18"/>
-      <c r="CQ1" s="18"/>
-      <c r="CR1" s="18"/>
-      <c r="CS1" s="18"/>
-      <c r="CT1" s="18"/>
-      <c r="CU1" s="18"/>
-      <c r="CV1" s="18"/>
-      <c r="CW1" s="18"/>
-      <c r="CX1" s="18"/>
-      <c r="CY1" s="18"/>
-      <c r="CZ1" s="18"/>
-      <c r="DA1" s="18"/>
-      <c r="DB1" s="18"/>
-      <c r="DC1" s="18"/>
-      <c r="DD1" s="18"/>
-      <c r="DE1" s="18"/>
-      <c r="DF1" s="18"/>
-      <c r="DG1" s="18"/>
-      <c r="DH1" s="18"/>
-      <c r="DI1" s="18"/>
-      <c r="DJ1" s="18"/>
-      <c r="DK1" s="18"/>
-      <c r="DL1" s="18"/>
-      <c r="DM1" s="18"/>
-      <c r="DN1" s="18"/>
-      <c r="DO1" s="18"/>
-      <c r="DP1" s="18"/>
-      <c r="DQ1" s="18"/>
-      <c r="DR1" s="18"/>
-      <c r="DS1" s="18"/>
-      <c r="DT1" s="18"/>
-      <c r="DU1" s="18"/>
-      <c r="DV1" s="18"/>
-      <c r="DW1" s="18"/>
-      <c r="DX1" s="18"/>
-      <c r="DY1" s="18"/>
-      <c r="DZ1" s="18"/>
-      <c r="EA1" s="18"/>
-      <c r="EB1" s="18"/>
-      <c r="EC1" s="18"/>
-      <c r="ED1" s="18"/>
-      <c r="EE1" s="18"/>
-      <c r="EF1" s="18"/>
-      <c r="EG1" s="18"/>
-      <c r="EH1" s="18"/>
-      <c r="EI1" s="18"/>
-      <c r="EJ1" s="18"/>
-      <c r="EK1" s="18"/>
-      <c r="EL1" s="18"/>
-      <c r="EM1" s="18"/>
-      <c r="EN1" s="18"/>
-      <c r="EO1" s="18"/>
-      <c r="EP1" s="18"/>
-      <c r="EQ1" s="18"/>
-      <c r="ER1" s="18"/>
-      <c r="ES1" s="18"/>
-      <c r="ET1" s="18"/>
-      <c r="EU1" s="18"/>
-      <c r="EV1" s="18"/>
-      <c r="EW1" s="18"/>
-      <c r="EX1" s="18"/>
-      <c r="EY1" s="18"/>
-      <c r="EZ1" s="18"/>
-      <c r="FA1" s="18"/>
-      <c r="FB1" s="18"/>
-      <c r="FC1" s="18"/>
-      <c r="FD1" s="18"/>
-      <c r="FE1" s="18"/>
-      <c r="FF1" s="18"/>
-      <c r="FG1" s="18"/>
-      <c r="FH1" s="18"/>
-      <c r="FI1" s="18"/>
-      <c r="FJ1" s="18"/>
-      <c r="FK1" s="18"/>
-      <c r="FL1" s="18"/>
-      <c r="FM1" s="18"/>
-      <c r="FN1" s="18"/>
-      <c r="FO1" s="18"/>
-      <c r="FP1" s="18"/>
-      <c r="FQ1" s="18"/>
-      <c r="FR1" s="18"/>
-      <c r="FS1" s="18"/>
-      <c r="FT1" s="18"/>
-      <c r="FU1" s="18"/>
-      <c r="FV1" s="18"/>
-      <c r="FW1" s="18"/>
-      <c r="FX1" s="18"/>
-      <c r="FY1" s="18"/>
-      <c r="FZ1" s="18"/>
-      <c r="GA1" s="18"/>
-      <c r="GB1" s="18"/>
-      <c r="GC1" s="18"/>
-      <c r="GD1" s="18"/>
-      <c r="GE1" s="18"/>
-      <c r="GF1" s="18"/>
-      <c r="GG1" s="18"/>
-      <c r="GH1" s="18"/>
-      <c r="GI1" s="18"/>
-      <c r="GJ1" s="18"/>
-      <c r="GK1" s="18"/>
-      <c r="GL1" s="18"/>
-      <c r="GM1" s="18"/>
-      <c r="GN1" s="18"/>
-      <c r="GO1" s="18"/>
-      <c r="GP1" s="18"/>
-      <c r="GQ1" s="18"/>
-      <c r="GR1" s="18"/>
-      <c r="GS1" s="18"/>
-      <c r="GT1" s="18"/>
-      <c r="GU1" s="18"/>
-      <c r="GV1" s="18"/>
-      <c r="GW1" s="18"/>
-      <c r="GX1" s="18"/>
-      <c r="GY1" s="18"/>
-      <c r="GZ1" s="18"/>
-      <c r="HA1" s="18"/>
-      <c r="HB1" s="18"/>
-      <c r="HC1" s="18"/>
-      <c r="HD1" s="18"/>
-      <c r="HE1" s="18"/>
-      <c r="HF1" s="18"/>
-      <c r="HG1" s="18"/>
-      <c r="HH1" s="18"/>
-      <c r="HI1" s="18"/>
-      <c r="HJ1" s="18"/>
-      <c r="HK1" s="18"/>
-      <c r="HL1" s="18"/>
-      <c r="HM1" s="18"/>
-      <c r="HN1" s="18"/>
-      <c r="HO1" s="18"/>
-      <c r="HP1" s="18"/>
-      <c r="HQ1" s="18"/>
-      <c r="HR1" s="18"/>
-      <c r="HS1" s="18"/>
-      <c r="HT1" s="18"/>
-      <c r="HU1" s="18"/>
-      <c r="HV1" s="18"/>
-      <c r="HW1" s="18"/>
-      <c r="HX1" s="18"/>
-      <c r="HY1" s="18"/>
-      <c r="HZ1" s="18"/>
-      <c r="IA1" s="18"/>
-      <c r="IB1" s="18"/>
-      <c r="IC1" s="18"/>
-      <c r="ID1" s="18"/>
-      <c r="IE1" s="18"/>
-      <c r="IF1" s="18"/>
-      <c r="IG1" s="18"/>
-      <c r="IH1" s="18"/>
-      <c r="II1" s="18"/>
-      <c r="IJ1" s="18"/>
-      <c r="IK1" s="18"/>
-      <c r="IL1" s="18"/>
-      <c r="IM1" s="18"/>
-      <c r="IN1" s="18"/>
-      <c r="IO1" s="18"/>
-      <c r="IP1" s="18"/>
-      <c r="IQ1" s="18"/>
-      <c r="IR1" s="18"/>
-      <c r="IS1" s="18"/>
-      <c r="IT1" s="18"/>
-      <c r="IU1" s="18"/>
-      <c r="IV1" s="18"/>
-      <c r="IW1" s="18"/>
-      <c r="IX1" s="18"/>
-      <c r="IY1" s="18"/>
-      <c r="IZ1" s="18"/>
-      <c r="JA1" s="18"/>
-      <c r="JB1" s="18"/>
-      <c r="JC1" s="18"/>
-      <c r="JD1" s="18"/>
-      <c r="JE1" s="18"/>
-      <c r="JF1" s="18"/>
-      <c r="JG1" s="18"/>
-      <c r="JH1" s="18"/>
-      <c r="JI1" s="18"/>
-      <c r="JJ1" s="18"/>
-      <c r="JK1" s="18"/>
-      <c r="JL1" s="18"/>
-      <c r="JM1" s="18"/>
-      <c r="JN1" s="18"/>
-      <c r="JO1" s="18"/>
-      <c r="JP1" s="18"/>
-      <c r="JQ1" s="18"/>
-      <c r="JR1" s="18"/>
-      <c r="JS1" s="18"/>
-      <c r="JT1" s="18"/>
-      <c r="JU1" s="18"/>
-      <c r="JV1" s="18"/>
-      <c r="JW1" s="18"/>
-      <c r="JX1" s="18"/>
-      <c r="JY1" s="18"/>
-      <c r="JZ1" s="18"/>
-      <c r="KA1" s="18"/>
-      <c r="KB1" s="18"/>
-      <c r="KC1" s="18"/>
-      <c r="KD1" s="18"/>
-      <c r="KE1" s="18"/>
-      <c r="KF1" s="18"/>
-      <c r="KG1" s="18"/>
-      <c r="KH1" s="18"/>
-      <c r="KI1" s="18"/>
-      <c r="KJ1" s="18"/>
-      <c r="KK1" s="18"/>
-      <c r="KL1" s="18"/>
-      <c r="KM1" s="18"/>
-      <c r="KN1" s="18"/>
-      <c r="KO1" s="18"/>
-      <c r="KP1" s="18"/>
-      <c r="KQ1" s="18"/>
-      <c r="KR1" s="18"/>
-      <c r="KS1" s="18"/>
-      <c r="KT1" s="18"/>
-      <c r="KU1" s="18"/>
-      <c r="KV1" s="18"/>
-      <c r="KW1" s="18"/>
-      <c r="KX1" s="18"/>
-      <c r="KY1" s="18"/>
-      <c r="KZ1" s="18"/>
-      <c r="LA1" s="18"/>
-      <c r="LB1" s="18"/>
-      <c r="LC1" s="18"/>
-      <c r="LD1" s="18"/>
-      <c r="LE1" s="18"/>
-      <c r="LF1" s="18"/>
-      <c r="LG1" s="18"/>
-      <c r="LH1" s="18"/>
-      <c r="LI1" s="18"/>
-      <c r="LJ1" s="18"/>
-      <c r="LK1" s="18"/>
-      <c r="LL1" s="18"/>
-      <c r="LM1" s="18"/>
-      <c r="LN1" s="18"/>
-      <c r="LO1" s="18"/>
-      <c r="LP1" s="18"/>
-      <c r="LQ1" s="18"/>
-      <c r="LR1" s="18"/>
-      <c r="LS1" s="18"/>
-      <c r="LT1" s="18"/>
-      <c r="LU1" s="18"/>
-      <c r="LV1" s="18"/>
-      <c r="LW1" s="18"/>
-      <c r="LX1" s="18"/>
-      <c r="LY1" s="18"/>
-      <c r="LZ1" s="18"/>
-      <c r="MA1" s="18"/>
-      <c r="MB1" s="18"/>
-      <c r="MC1" s="18"/>
-      <c r="MD1" s="18"/>
-      <c r="ME1" s="18"/>
-      <c r="MF1" s="18"/>
-      <c r="MG1" s="18"/>
-      <c r="MH1" s="18"/>
-      <c r="MI1" s="18"/>
-      <c r="MJ1" s="18"/>
-      <c r="MK1" s="18"/>
-      <c r="ML1" s="18"/>
-      <c r="MM1" s="18"/>
-      <c r="MN1" s="18"/>
-      <c r="MO1" s="18"/>
-      <c r="MP1" s="18"/>
-      <c r="MQ1" s="18"/>
-      <c r="MR1" s="18"/>
-      <c r="MS1" s="18"/>
-      <c r="MT1" s="18"/>
-      <c r="MU1" s="18"/>
-      <c r="MV1" s="18"/>
-      <c r="MW1" s="18"/>
-      <c r="MX1" s="18"/>
-      <c r="MY1" s="18"/>
-      <c r="MZ1" s="18"/>
-      <c r="NA1" s="18"/>
-      <c r="NB1" s="18"/>
-      <c r="NC1" s="18"/>
-      <c r="ND1" s="18"/>
-      <c r="NE1" s="18"/>
-      <c r="NF1" s="18"/>
-      <c r="NG1" s="18"/>
-      <c r="NH1" s="18"/>
-      <c r="NI1" s="18"/>
-      <c r="NJ1" s="18"/>
-      <c r="NK1" s="18"/>
-      <c r="NL1" s="18"/>
-      <c r="NM1" s="18"/>
-      <c r="NN1" s="18"/>
-      <c r="NO1" s="18"/>
-      <c r="NP1" s="18"/>
-      <c r="NQ1" s="18"/>
-      <c r="NR1" s="18"/>
-      <c r="NS1" s="18"/>
-      <c r="NT1" s="18"/>
-      <c r="NU1" s="18"/>
-      <c r="NV1" s="18"/>
-      <c r="NW1" s="18"/>
-      <c r="NX1" s="18"/>
-      <c r="NY1" s="18"/>
-      <c r="NZ1" s="18"/>
-      <c r="OA1" s="18"/>
-      <c r="OB1" s="18"/>
-      <c r="OC1" s="18"/>
-      <c r="OD1" s="18"/>
-      <c r="OE1" s="18"/>
-      <c r="OF1" s="18"/>
-      <c r="OG1" s="18"/>
-      <c r="OH1" s="18"/>
-      <c r="OI1" s="18"/>
-      <c r="OJ1" s="18"/>
-      <c r="OK1" s="18"/>
-      <c r="OL1" s="18"/>
-      <c r="OM1" s="18"/>
-      <c r="ON1" s="18"/>
-      <c r="OO1" s="18"/>
-      <c r="OP1" s="18"/>
-      <c r="OQ1" s="18"/>
-      <c r="OR1" s="18"/>
-      <c r="OS1" s="18"/>
-      <c r="OT1" s="18"/>
-      <c r="OU1" s="18"/>
-      <c r="OV1" s="18"/>
-      <c r="OW1" s="18"/>
-      <c r="OX1" s="18"/>
-      <c r="OY1" s="18"/>
-      <c r="OZ1" s="18"/>
-      <c r="PA1" s="18"/>
-      <c r="PB1" s="18"/>
-      <c r="PC1" s="18"/>
-      <c r="PD1" s="18"/>
-      <c r="PE1" s="18"/>
-      <c r="PF1" s="18"/>
-      <c r="PG1" s="18"/>
-      <c r="PH1" s="18"/>
-      <c r="PI1" s="18"/>
-      <c r="PJ1" s="18"/>
-      <c r="PK1" s="18"/>
-      <c r="PL1" s="18"/>
-      <c r="PM1" s="18"/>
-      <c r="PN1" s="18"/>
-      <c r="PO1" s="18"/>
-      <c r="PP1" s="18"/>
-      <c r="PQ1" s="18"/>
-      <c r="PR1" s="18"/>
-      <c r="PS1" s="18"/>
-      <c r="PT1" s="18"/>
-      <c r="PU1" s="18"/>
-      <c r="PV1" s="18"/>
-      <c r="PW1" s="18"/>
-      <c r="PX1" s="18"/>
-      <c r="PY1" s="18"/>
-      <c r="PZ1" s="18"/>
-      <c r="QA1" s="18"/>
-      <c r="QB1" s="18"/>
-      <c r="QC1" s="18"/>
-      <c r="QD1" s="18"/>
-      <c r="QE1" s="18"/>
-      <c r="QF1" s="18"/>
-      <c r="QG1" s="18"/>
-      <c r="QH1" s="18"/>
-      <c r="QI1" s="18"/>
-      <c r="QJ1" s="18"/>
-      <c r="QK1" s="18"/>
-      <c r="QL1" s="18"/>
-      <c r="QM1" s="18"/>
-      <c r="QN1" s="18"/>
-      <c r="QO1" s="18"/>
-      <c r="QP1" s="18"/>
-      <c r="QQ1" s="18"/>
-      <c r="QR1" s="18"/>
-      <c r="QS1" s="18"/>
-      <c r="QT1" s="18"/>
-      <c r="QU1" s="18"/>
-      <c r="QV1" s="18"/>
-      <c r="QW1" s="18"/>
-      <c r="QX1" s="18"/>
-      <c r="QY1" s="18"/>
-      <c r="QZ1" s="18"/>
-      <c r="RA1" s="18"/>
-      <c r="RB1" s="18"/>
-      <c r="RC1" s="18"/>
-      <c r="RD1" s="18"/>
-      <c r="RE1" s="18"/>
-      <c r="RF1" s="18"/>
-      <c r="RG1" s="18"/>
-      <c r="RH1" s="18"/>
-      <c r="RI1" s="18"/>
-      <c r="RJ1" s="18"/>
-      <c r="RK1" s="18"/>
-      <c r="RL1" s="18"/>
-      <c r="RM1" s="18"/>
-      <c r="RN1" s="18"/>
-      <c r="RO1" s="18"/>
-      <c r="RP1" s="18"/>
-      <c r="RQ1" s="18"/>
-      <c r="RR1" s="18"/>
-      <c r="RS1" s="18"/>
-      <c r="RT1" s="18"/>
-      <c r="RU1" s="18"/>
-      <c r="RV1" s="18"/>
-      <c r="RW1" s="18"/>
-      <c r="RX1" s="18"/>
-      <c r="RY1" s="18"/>
-      <c r="RZ1" s="18"/>
-      <c r="SA1" s="18"/>
-      <c r="SB1" s="18"/>
-      <c r="SC1" s="18"/>
-      <c r="SD1" s="18"/>
-      <c r="SE1" s="18"/>
-      <c r="SF1" s="18"/>
-      <c r="SG1" s="18"/>
-      <c r="SH1" s="18"/>
-      <c r="SI1" s="18"/>
-      <c r="SJ1" s="18"/>
-      <c r="SK1" s="18"/>
-      <c r="SL1" s="18"/>
-      <c r="SM1" s="18"/>
-      <c r="SN1" s="18"/>
-      <c r="SO1" s="18"/>
-      <c r="SP1" s="18"/>
-      <c r="SQ1" s="18"/>
-      <c r="SR1" s="18"/>
-      <c r="SS1" s="18"/>
-      <c r="ST1" s="18"/>
-      <c r="SU1" s="18"/>
-      <c r="SV1" s="18"/>
-      <c r="SW1" s="18"/>
-      <c r="SX1" s="18"/>
-      <c r="SY1" s="18"/>
-      <c r="SZ1" s="18"/>
-      <c r="TA1" s="18"/>
-      <c r="TB1" s="18"/>
-      <c r="TC1" s="18"/>
-      <c r="TD1" s="18"/>
-      <c r="TE1" s="18"/>
-      <c r="TF1" s="18"/>
-      <c r="TG1" s="18"/>
-      <c r="TH1" s="18"/>
-      <c r="TI1" s="18"/>
-      <c r="TJ1" s="18"/>
-      <c r="TK1" s="18"/>
-      <c r="TL1" s="18"/>
-      <c r="TM1" s="18"/>
-      <c r="TN1" s="18"/>
-      <c r="TO1" s="18"/>
-      <c r="TP1" s="18"/>
-      <c r="TQ1" s="18"/>
-      <c r="TR1" s="18"/>
-      <c r="TS1" s="18"/>
-      <c r="TT1" s="18"/>
-      <c r="TU1" s="18"/>
-      <c r="TV1" s="18"/>
-      <c r="TW1" s="18"/>
-      <c r="TX1" s="18"/>
-      <c r="TY1" s="18"/>
-      <c r="TZ1" s="18"/>
-      <c r="UA1" s="18"/>
-      <c r="UB1" s="18"/>
-      <c r="UC1" s="18"/>
-      <c r="UD1" s="18"/>
-      <c r="UE1" s="18"/>
-      <c r="UF1" s="18"/>
-      <c r="UG1" s="18"/>
-      <c r="UH1" s="18"/>
-      <c r="UI1" s="18"/>
-      <c r="UJ1" s="18"/>
-      <c r="UK1" s="18"/>
-      <c r="UL1" s="18"/>
-      <c r="UM1" s="18"/>
-      <c r="UN1" s="18"/>
-      <c r="UO1" s="18"/>
-      <c r="UP1" s="18"/>
-      <c r="UQ1" s="18"/>
-      <c r="UR1" s="18"/>
-      <c r="US1" s="18"/>
-      <c r="UT1" s="18"/>
-      <c r="UU1" s="18"/>
-      <c r="UV1" s="18"/>
-      <c r="UW1" s="18"/>
-      <c r="UX1" s="18"/>
-      <c r="UY1" s="18"/>
-      <c r="UZ1" s="18"/>
-      <c r="VA1" s="18"/>
-      <c r="VB1" s="18"/>
-      <c r="VC1" s="18"/>
-      <c r="VD1" s="18"/>
-      <c r="VE1" s="18"/>
-      <c r="VF1" s="18"/>
-      <c r="VG1" s="18"/>
-      <c r="VH1" s="18"/>
-      <c r="VI1" s="18"/>
-      <c r="VJ1" s="18"/>
-      <c r="VK1" s="18"/>
-      <c r="VL1" s="18"/>
-      <c r="VM1" s="18"/>
-      <c r="VN1" s="18"/>
-      <c r="VO1" s="18"/>
-      <c r="VP1" s="18"/>
-      <c r="VQ1" s="18"/>
-      <c r="VR1" s="18"/>
-      <c r="VS1" s="18"/>
-      <c r="VT1" s="18"/>
-      <c r="VU1" s="18"/>
-      <c r="VV1" s="18"/>
-      <c r="VW1" s="18"/>
-      <c r="VX1" s="18"/>
-      <c r="VY1" s="18"/>
-      <c r="VZ1" s="18"/>
-      <c r="WA1" s="18"/>
-      <c r="WB1" s="18"/>
-      <c r="WC1" s="18"/>
-      <c r="WD1" s="18"/>
-      <c r="WE1" s="18"/>
-      <c r="WF1" s="18"/>
-      <c r="WG1" s="18"/>
-      <c r="WH1" s="18"/>
-      <c r="WI1" s="18"/>
-      <c r="WJ1" s="18"/>
-      <c r="WK1" s="18"/>
-      <c r="WL1" s="18"/>
-      <c r="WM1" s="18"/>
-      <c r="WN1" s="18"/>
-      <c r="WO1" s="18"/>
-      <c r="WP1" s="18"/>
-      <c r="WQ1" s="18"/>
-      <c r="WR1" s="18"/>
-      <c r="WS1" s="18"/>
-      <c r="WT1" s="18"/>
-      <c r="WU1" s="18"/>
-      <c r="WV1" s="18"/>
-      <c r="WW1" s="18"/>
-      <c r="WX1" s="18"/>
-      <c r="WY1" s="18"/>
-      <c r="WZ1" s="18"/>
-      <c r="XA1" s="18"/>
-      <c r="XB1" s="18"/>
-      <c r="XC1" s="18"/>
-      <c r="XD1" s="18"/>
-      <c r="XE1" s="18"/>
-      <c r="XF1" s="18"/>
-      <c r="XG1" s="18"/>
-      <c r="XH1" s="18"/>
-      <c r="XI1" s="18"/>
-      <c r="XJ1" s="18"/>
-      <c r="XK1" s="18"/>
-      <c r="XL1" s="18"/>
-      <c r="XM1" s="18"/>
-      <c r="XN1" s="18"/>
-      <c r="XO1" s="18"/>
-      <c r="XP1" s="18"/>
-      <c r="XQ1" s="18"/>
-      <c r="XR1" s="18"/>
-      <c r="XS1" s="18"/>
-      <c r="XT1" s="18"/>
-      <c r="XU1" s="18"/>
-      <c r="XV1" s="18"/>
-      <c r="XW1" s="18"/>
-      <c r="XX1" s="18"/>
-      <c r="XY1" s="18"/>
-      <c r="XZ1" s="18"/>
-      <c r="YA1" s="18"/>
-      <c r="YB1" s="18"/>
-      <c r="YC1" s="18"/>
-      <c r="YD1" s="18"/>
-      <c r="YE1" s="18"/>
-      <c r="YF1" s="18"/>
-      <c r="YG1" s="18"/>
-      <c r="YH1" s="18"/>
-      <c r="YI1" s="18"/>
-      <c r="YJ1" s="18"/>
-      <c r="YK1" s="18"/>
-      <c r="YL1" s="18"/>
-      <c r="YM1" s="18"/>
-      <c r="YN1" s="18"/>
-      <c r="YO1" s="18"/>
-      <c r="YP1" s="18"/>
-      <c r="YQ1" s="18"/>
-      <c r="YR1" s="18"/>
-      <c r="YS1" s="18"/>
-      <c r="YT1" s="18"/>
-      <c r="YU1" s="18"/>
-      <c r="YV1" s="18"/>
-      <c r="YW1" s="18"/>
-      <c r="YX1" s="18"/>
-      <c r="YY1" s="18"/>
-      <c r="YZ1" s="18"/>
-      <c r="ZA1" s="18"/>
-      <c r="ZB1" s="18"/>
-      <c r="ZC1" s="18"/>
-      <c r="ZD1" s="18"/>
-      <c r="ZE1" s="18"/>
-      <c r="ZF1" s="18"/>
-      <c r="ZG1" s="18"/>
-      <c r="ZH1" s="18"/>
-      <c r="ZI1" s="18"/>
-      <c r="ZJ1" s="18"/>
-      <c r="ZK1" s="18"/>
-      <c r="ZL1" s="18"/>
-      <c r="ZM1" s="18"/>
-      <c r="ZN1" s="18"/>
-      <c r="ZO1" s="18"/>
-      <c r="ZP1" s="18"/>
-      <c r="ZQ1" s="18"/>
-      <c r="ZR1" s="18"/>
-      <c r="ZS1" s="18"/>
-      <c r="ZT1" s="18"/>
-      <c r="ZU1" s="18"/>
-      <c r="ZV1" s="18"/>
-      <c r="ZW1" s="18"/>
-      <c r="ZX1" s="18"/>
-      <c r="ZY1" s="18"/>
-      <c r="ZZ1" s="18"/>
-      <c r="AAA1" s="18"/>
-      <c r="AAB1" s="18"/>
-      <c r="AAC1" s="18"/>
-      <c r="AAD1" s="18"/>
-      <c r="AAE1" s="18"/>
-      <c r="AAF1" s="18"/>
-      <c r="AAG1" s="18"/>
-      <c r="AAH1" s="18"/>
-      <c r="AAI1" s="18"/>
-      <c r="AAJ1" s="18"/>
-      <c r="AAK1" s="18"/>
-      <c r="AAL1" s="18"/>
-      <c r="AAM1" s="18"/>
-      <c r="AAN1" s="18"/>
-      <c r="AAO1" s="18"/>
-      <c r="AAP1" s="18"/>
-      <c r="AAQ1" s="18"/>
-      <c r="AAR1" s="18"/>
-      <c r="AAS1" s="18"/>
-      <c r="AAT1" s="18"/>
-      <c r="AAU1" s="18"/>
-      <c r="AAV1" s="18"/>
-      <c r="AAW1" s="18"/>
-      <c r="AAX1" s="18"/>
-      <c r="AAY1" s="18"/>
-      <c r="AAZ1" s="18"/>
-      <c r="ABA1" s="18"/>
-      <c r="ABB1" s="18"/>
-      <c r="ABC1" s="18"/>
-      <c r="ABD1" s="18"/>
-      <c r="ABE1" s="18"/>
-      <c r="ABF1" s="18"/>
-      <c r="ABG1" s="18"/>
-      <c r="ABH1" s="18"/>
-      <c r="ABI1" s="18"/>
-      <c r="ABJ1" s="18"/>
-      <c r="ABK1" s="18"/>
-      <c r="ABL1" s="18"/>
-      <c r="ABM1" s="18"/>
-      <c r="ABN1" s="18"/>
-      <c r="ABO1" s="18"/>
-      <c r="ABP1" s="18"/>
-      <c r="ABQ1" s="18"/>
-      <c r="ABR1" s="18"/>
-      <c r="ABS1" s="18"/>
-      <c r="ABT1" s="18"/>
-      <c r="ABU1" s="18"/>
-      <c r="ABV1" s="18"/>
-      <c r="ABW1" s="18"/>
-      <c r="ABX1" s="18"/>
-      <c r="ABY1" s="18"/>
-      <c r="ABZ1" s="18"/>
-      <c r="ACA1" s="18"/>
-      <c r="ACB1" s="18"/>
-      <c r="ACC1" s="18"/>
-      <c r="ACD1" s="18"/>
-      <c r="ACE1" s="18"/>
-      <c r="ACF1" s="18"/>
-      <c r="ACG1" s="18"/>
-      <c r="ACH1" s="18"/>
-      <c r="ACI1" s="18"/>
-      <c r="ACJ1" s="18"/>
-      <c r="ACK1" s="18"/>
-      <c r="ACL1" s="18"/>
-      <c r="ACM1" s="18"/>
-      <c r="ACN1" s="18"/>
-      <c r="ACO1" s="18"/>
-      <c r="ACP1" s="18"/>
-      <c r="ACQ1" s="18"/>
-      <c r="ACR1" s="18"/>
-      <c r="ACS1" s="18"/>
-      <c r="ACT1" s="18"/>
-      <c r="ACU1" s="18"/>
-      <c r="ACV1" s="18"/>
-      <c r="ACW1" s="18"/>
-      <c r="ACX1" s="18"/>
-      <c r="ACY1" s="18"/>
-      <c r="ACZ1" s="18"/>
-      <c r="ADA1" s="18"/>
-      <c r="ADB1" s="18"/>
-      <c r="ADC1" s="18"/>
-      <c r="ADD1" s="18"/>
-      <c r="ADE1" s="18"/>
-      <c r="ADF1" s="18"/>
-      <c r="ADG1" s="18"/>
-      <c r="ADH1" s="18"/>
-      <c r="ADI1" s="18"/>
-      <c r="ADJ1" s="18"/>
-      <c r="ADK1" s="18"/>
-      <c r="ADL1" s="18"/>
-      <c r="ADM1" s="18"/>
-      <c r="ADN1" s="18"/>
-      <c r="ADO1" s="18"/>
-      <c r="ADP1" s="18"/>
-      <c r="ADQ1" s="18"/>
-      <c r="ADR1" s="18"/>
-      <c r="ADS1" s="18"/>
-      <c r="ADT1" s="18"/>
-      <c r="ADU1" s="18"/>
-      <c r="ADV1" s="18"/>
-      <c r="ADW1" s="18"/>
-      <c r="ADX1" s="18"/>
-      <c r="ADY1" s="18"/>
-      <c r="ADZ1" s="18"/>
-      <c r="AEA1" s="18"/>
-      <c r="AEB1" s="18"/>
-      <c r="AEC1" s="18"/>
-      <c r="AED1" s="18"/>
-      <c r="AEE1" s="18"/>
-      <c r="AEF1" s="18"/>
-      <c r="AEG1" s="18"/>
-      <c r="AEH1" s="18"/>
-      <c r="AEI1" s="18"/>
-      <c r="AEJ1" s="18"/>
-      <c r="AEK1" s="18"/>
-      <c r="AEL1" s="18"/>
-      <c r="AEM1" s="18"/>
-      <c r="AEN1" s="18"/>
-      <c r="AEO1" s="18"/>
-      <c r="AEP1" s="18"/>
-      <c r="AEQ1" s="18"/>
-      <c r="AER1" s="18"/>
-      <c r="AES1" s="18"/>
-      <c r="AET1" s="18"/>
-      <c r="AEU1" s="18"/>
-      <c r="AEV1" s="18"/>
-      <c r="AEW1" s="18"/>
-      <c r="AEX1" s="18"/>
-      <c r="AEY1" s="18"/>
-      <c r="AEZ1" s="18"/>
-      <c r="AFA1" s="18"/>
-      <c r="AFB1" s="18"/>
-      <c r="AFC1" s="18"/>
-      <c r="AFD1" s="18"/>
-      <c r="AFE1" s="18"/>
-      <c r="AFF1" s="18"/>
-      <c r="AFG1" s="18"/>
-      <c r="AFH1" s="18"/>
-      <c r="AFI1" s="18"/>
-      <c r="AFJ1" s="18"/>
-      <c r="AFK1" s="18"/>
-      <c r="AFL1" s="18"/>
-      <c r="AFM1" s="18"/>
-      <c r="AFN1" s="18"/>
-      <c r="AFO1" s="18"/>
-      <c r="AFP1" s="18"/>
-      <c r="AFQ1" s="18"/>
-      <c r="AFR1" s="18"/>
-      <c r="AFS1" s="18"/>
-      <c r="AFT1" s="18"/>
-      <c r="AFU1" s="18"/>
-      <c r="AFV1" s="18"/>
-      <c r="AFW1" s="18"/>
-      <c r="AFX1" s="18"/>
-      <c r="AFY1" s="18"/>
-      <c r="AFZ1" s="18"/>
-      <c r="AGA1" s="18"/>
-      <c r="AGB1" s="18"/>
-      <c r="AGC1" s="18"/>
-      <c r="AGD1" s="18"/>
-      <c r="AGE1" s="18"/>
-      <c r="AGF1" s="18"/>
-      <c r="AGG1" s="18"/>
-      <c r="AGH1" s="18"/>
-      <c r="AGI1" s="18"/>
-      <c r="AGJ1" s="18"/>
-      <c r="AGK1" s="18"/>
-      <c r="AGL1" s="18"/>
-      <c r="AGM1" s="18"/>
-      <c r="AGN1" s="18"/>
-      <c r="AGO1" s="18"/>
-      <c r="AGP1" s="18"/>
-      <c r="AGQ1" s="18"/>
-      <c r="AGR1" s="18"/>
-      <c r="AGS1" s="18"/>
-      <c r="AGT1" s="18"/>
-      <c r="AGU1" s="18"/>
-      <c r="AGV1" s="18"/>
-      <c r="AGW1" s="18"/>
-      <c r="AGX1" s="18"/>
-      <c r="AGY1" s="18"/>
-      <c r="AGZ1" s="18"/>
-      <c r="AHA1" s="18"/>
-      <c r="AHB1" s="18"/>
-      <c r="AHC1" s="18"/>
-      <c r="AHD1" s="18"/>
-      <c r="AHE1" s="18"/>
-      <c r="AHF1" s="18"/>
-      <c r="AHG1" s="18"/>
-      <c r="AHH1" s="18"/>
-      <c r="AHI1" s="18"/>
-      <c r="AHJ1" s="18"/>
-      <c r="AHK1" s="18"/>
-      <c r="AHL1" s="18"/>
-      <c r="AHM1" s="18"/>
-      <c r="AHN1" s="18"/>
-      <c r="AHO1" s="18"/>
-      <c r="AHP1" s="18"/>
-      <c r="AHQ1" s="18"/>
-      <c r="AHR1" s="18"/>
-      <c r="AHS1" s="18"/>
-      <c r="AHT1" s="18"/>
-      <c r="AHU1" s="18"/>
-      <c r="AHV1" s="18"/>
-      <c r="AHW1" s="18"/>
-      <c r="AHX1" s="18"/>
-      <c r="AHY1" s="18"/>
-      <c r="AHZ1" s="18"/>
-      <c r="AIA1" s="18"/>
-      <c r="AIB1" s="18"/>
-      <c r="AIC1" s="18"/>
-      <c r="AID1" s="18"/>
-      <c r="AIE1" s="18"/>
-      <c r="AIF1" s="18"/>
-      <c r="AIG1" s="18"/>
-      <c r="AIH1" s="18"/>
-      <c r="AII1" s="18"/>
-      <c r="AIJ1" s="18"/>
-      <c r="AIK1" s="18"/>
-      <c r="AIL1" s="18"/>
-      <c r="AIM1" s="18"/>
-      <c r="AIN1" s="18"/>
-      <c r="AIO1" s="18"/>
-      <c r="AIP1" s="18"/>
-      <c r="AIQ1" s="18"/>
-      <c r="AIR1" s="18"/>
-      <c r="AIS1" s="18"/>
-      <c r="AIT1" s="18"/>
-      <c r="AIU1" s="18"/>
-      <c r="AIV1" s="18"/>
-      <c r="AIW1" s="18"/>
-      <c r="AIX1" s="18"/>
-      <c r="AIY1" s="18"/>
-      <c r="AIZ1" s="18"/>
-      <c r="AJA1" s="18"/>
-      <c r="AJB1" s="18"/>
-      <c r="AJC1" s="18"/>
-      <c r="AJD1" s="18"/>
-      <c r="AJE1" s="18"/>
-      <c r="AJF1" s="18"/>
-      <c r="AJG1" s="18"/>
-      <c r="AJH1" s="18"/>
-      <c r="AJI1" s="18"/>
-      <c r="AJJ1" s="18"/>
-      <c r="AJK1" s="18"/>
-      <c r="AJL1" s="18"/>
-      <c r="AJM1" s="18"/>
-      <c r="AJN1" s="18"/>
-      <c r="AJO1" s="18"/>
-      <c r="AJP1" s="18"/>
-      <c r="AJQ1" s="18"/>
-      <c r="AJR1" s="18"/>
-      <c r="AJS1" s="18"/>
-      <c r="AJT1" s="18"/>
-      <c r="AJU1" s="18"/>
-      <c r="AJV1" s="18"/>
-      <c r="AJW1" s="18"/>
-      <c r="AJX1" s="18"/>
-      <c r="AJY1" s="18"/>
-      <c r="AJZ1" s="18"/>
-      <c r="AKA1" s="18"/>
-      <c r="AKB1" s="18"/>
-      <c r="AKC1" s="18"/>
-      <c r="AKD1" s="18"/>
-      <c r="AKE1" s="18"/>
-      <c r="AKF1" s="18"/>
-      <c r="AKG1" s="18"/>
-      <c r="AKH1" s="18"/>
-      <c r="AKI1" s="18"/>
-      <c r="AKJ1" s="18"/>
-      <c r="AKK1" s="18"/>
-      <c r="AKL1" s="18"/>
-      <c r="AKM1" s="18"/>
-      <c r="AKN1" s="18"/>
-      <c r="AKO1" s="18"/>
-      <c r="AKP1" s="18"/>
-      <c r="AKQ1" s="18"/>
-      <c r="AKR1" s="18"/>
-      <c r="AKS1" s="18"/>
-      <c r="AKT1" s="18"/>
-      <c r="AKU1" s="18"/>
-      <c r="AKV1" s="18"/>
-      <c r="AKW1" s="18"/>
-      <c r="AKX1" s="18"/>
-      <c r="AKY1" s="18"/>
-      <c r="AKZ1" s="18"/>
-      <c r="ALA1" s="18"/>
-      <c r="ALB1" s="18"/>
-      <c r="ALC1" s="18"/>
-      <c r="ALD1" s="18"/>
-      <c r="ALE1" s="18"/>
-      <c r="ALF1" s="18"/>
-      <c r="ALG1" s="18"/>
-      <c r="ALH1" s="18"/>
-      <c r="ALI1" s="18"/>
-      <c r="ALJ1" s="18"/>
-      <c r="ALK1" s="18"/>
-      <c r="ALL1" s="18"/>
-      <c r="ALM1" s="18"/>
-      <c r="ALN1" s="18"/>
-      <c r="ALO1" s="18"/>
-      <c r="ALP1" s="18"/>
-      <c r="ALQ1" s="18"/>
-      <c r="ALR1" s="18"/>
-      <c r="ALS1" s="18"/>
-      <c r="ALT1" s="18"/>
-      <c r="ALU1" s="18"/>
-      <c r="ALV1" s="18"/>
-      <c r="ALW1" s="18"/>
-      <c r="ALX1" s="18"/>
-      <c r="ALY1" s="18"/>
-      <c r="ALZ1" s="18"/>
-      <c r="AMA1" s="18"/>
-      <c r="AMB1" s="18"/>
-      <c r="AMC1" s="18"/>
-      <c r="AMD1" s="18"/>
-      <c r="AME1" s="18"/>
-      <c r="AMF1" s="18"/>
-      <c r="AMG1" s="18"/>
-      <c r="AMH1" s="18"/>
-      <c r="AMI1" s="18"/>
-      <c r="AMJ1" s="18"/>
-      <c r="AMK1" s="18"/>
-      <c r="AML1" s="18"/>
-      <c r="AMM1" s="18"/>
-      <c r="AMN1" s="18"/>
-      <c r="AMO1" s="18"/>
-      <c r="AMP1" s="18"/>
-      <c r="AMQ1"/>
-      <c r="AMR1"/>
+      <c r="N1" s="27"/>
+      <c r="O1" s="27"/>
+      <c r="P1" s="27"/>
+      <c r="Q1" s="17"/>
+      <c r="R1" s="17"/>
+      <c r="S1" s="17"/>
+      <c r="T1" s="17"/>
+      <c r="U1" s="17"/>
+      <c r="V1" s="17"/>
+      <c r="W1" s="17"/>
+      <c r="X1" s="17"/>
+      <c r="Y1" s="17"/>
+      <c r="Z1" s="17"/>
+      <c r="AA1" s="17"/>
+      <c r="AB1" s="17"/>
+      <c r="AC1" s="17"/>
+      <c r="AD1" s="17"/>
+      <c r="AE1" s="17"/>
+      <c r="AF1" s="17"/>
+      <c r="AG1" s="17"/>
+      <c r="AH1" s="17"/>
+      <c r="AI1" s="17"/>
+      <c r="AJ1" s="17"/>
+      <c r="AK1" s="17"/>
+      <c r="AL1" s="17"/>
+      <c r="AM1" s="17"/>
+      <c r="AN1" s="17"/>
+      <c r="AO1" s="17"/>
+      <c r="AP1" s="17"/>
+      <c r="AQ1" s="17"/>
+      <c r="AR1" s="17"/>
+      <c r="AS1" s="17"/>
+      <c r="AT1" s="17"/>
+      <c r="AU1" s="17"/>
+      <c r="AV1" s="17"/>
+      <c r="AW1" s="17"/>
+      <c r="AX1" s="17"/>
+      <c r="AY1" s="17"/>
+      <c r="AZ1" s="17"/>
+      <c r="BA1" s="17"/>
+      <c r="BB1" s="17"/>
+      <c r="BC1" s="17"/>
+      <c r="BD1" s="17"/>
+      <c r="BE1" s="17"/>
+      <c r="BF1" s="17"/>
+      <c r="BG1" s="17"/>
+      <c r="BH1" s="17"/>
+      <c r="BI1" s="17"/>
+      <c r="BJ1" s="17"/>
+      <c r="BK1" s="17"/>
+      <c r="BL1" s="17"/>
+      <c r="BM1" s="17"/>
+      <c r="BN1" s="17"/>
+      <c r="BO1" s="17"/>
+      <c r="BP1" s="17"/>
+      <c r="BQ1" s="17"/>
+      <c r="BR1" s="17"/>
+      <c r="BS1" s="17"/>
+      <c r="BT1" s="17"/>
+      <c r="BU1" s="17"/>
+      <c r="BV1" s="17"/>
+      <c r="BW1" s="17"/>
+      <c r="BX1" s="17"/>
+      <c r="BY1" s="17"/>
+      <c r="BZ1" s="17"/>
+      <c r="CA1" s="17"/>
+      <c r="CB1" s="17"/>
+      <c r="CC1" s="17"/>
+      <c r="CD1" s="17"/>
+      <c r="CE1" s="17"/>
+      <c r="CF1" s="17"/>
+      <c r="CG1" s="17"/>
+      <c r="CH1" s="17"/>
+      <c r="CI1" s="17"/>
+      <c r="CJ1" s="17"/>
+      <c r="CK1" s="17"/>
+      <c r="CL1" s="17"/>
+      <c r="CM1" s="17"/>
+      <c r="CN1" s="17"/>
+      <c r="CO1" s="17"/>
+      <c r="CP1" s="17"/>
+      <c r="CQ1" s="17"/>
+      <c r="CR1" s="17"/>
+      <c r="CS1" s="17"/>
+      <c r="CT1" s="17"/>
+      <c r="CU1" s="17"/>
+      <c r="CV1" s="17"/>
+      <c r="CW1" s="17"/>
+      <c r="CX1" s="17"/>
+      <c r="CY1" s="17"/>
+      <c r="CZ1" s="17"/>
+      <c r="DA1" s="17"/>
+      <c r="DB1" s="17"/>
+      <c r="DC1" s="17"/>
+      <c r="DD1" s="17"/>
+      <c r="DE1" s="17"/>
+      <c r="DF1" s="17"/>
+      <c r="DG1" s="17"/>
+      <c r="DH1" s="17"/>
+      <c r="DI1" s="17"/>
+      <c r="DJ1" s="17"/>
+      <c r="DK1" s="17"/>
+      <c r="DL1" s="17"/>
+      <c r="DM1" s="17"/>
+      <c r="DN1" s="17"/>
+      <c r="DO1" s="17"/>
+      <c r="DP1" s="17"/>
+      <c r="DQ1" s="17"/>
+      <c r="DR1" s="17"/>
+      <c r="DS1" s="17"/>
+      <c r="DT1" s="17"/>
+      <c r="DU1" s="17"/>
+      <c r="DV1" s="17"/>
+      <c r="DW1" s="17"/>
+      <c r="DX1" s="17"/>
+      <c r="DY1" s="17"/>
+      <c r="DZ1" s="17"/>
+      <c r="EA1" s="17"/>
+      <c r="EB1" s="17"/>
+      <c r="EC1" s="17"/>
+      <c r="ED1" s="17"/>
+      <c r="EE1" s="17"/>
+      <c r="EF1" s="17"/>
+      <c r="EG1" s="17"/>
+      <c r="EH1" s="17"/>
+      <c r="EI1" s="17"/>
+      <c r="EJ1" s="17"/>
+      <c r="EK1" s="17"/>
+      <c r="EL1" s="17"/>
+      <c r="EM1" s="17"/>
+      <c r="EN1" s="17"/>
+      <c r="EO1" s="17"/>
+      <c r="EP1" s="17"/>
+      <c r="EQ1" s="17"/>
+      <c r="ER1" s="17"/>
+      <c r="ES1" s="17"/>
+      <c r="ET1" s="17"/>
+      <c r="EU1" s="17"/>
+      <c r="EV1" s="17"/>
+      <c r="EW1" s="17"/>
+      <c r="EX1" s="17"/>
+      <c r="EY1" s="17"/>
+      <c r="EZ1" s="17"/>
+      <c r="FA1" s="17"/>
+      <c r="FB1" s="17"/>
+      <c r="FC1" s="17"/>
+      <c r="FD1" s="17"/>
+      <c r="FE1" s="17"/>
+      <c r="FF1" s="17"/>
+      <c r="FG1" s="17"/>
+      <c r="FH1" s="17"/>
+      <c r="FI1" s="17"/>
+      <c r="FJ1" s="17"/>
+      <c r="FK1" s="17"/>
+      <c r="FL1" s="17"/>
+      <c r="FM1" s="17"/>
+      <c r="FN1" s="17"/>
+      <c r="FO1" s="17"/>
+      <c r="FP1" s="17"/>
+      <c r="FQ1" s="17"/>
+      <c r="FR1" s="17"/>
+      <c r="FS1" s="17"/>
+      <c r="FT1" s="17"/>
+      <c r="FU1" s="17"/>
+      <c r="FV1" s="17"/>
+      <c r="FW1" s="17"/>
+      <c r="FX1" s="17"/>
+      <c r="FY1" s="17"/>
+      <c r="FZ1" s="17"/>
+      <c r="GA1" s="17"/>
+      <c r="GB1" s="17"/>
+      <c r="GC1" s="17"/>
+      <c r="GD1" s="17"/>
+      <c r="GE1" s="17"/>
+      <c r="GF1" s="17"/>
+      <c r="GG1" s="17"/>
+      <c r="GH1" s="17"/>
+      <c r="GI1" s="17"/>
+      <c r="GJ1" s="17"/>
+      <c r="GK1" s="17"/>
+      <c r="GL1" s="17"/>
+      <c r="GM1" s="17"/>
+      <c r="GN1" s="17"/>
+      <c r="GO1" s="17"/>
+      <c r="GP1" s="17"/>
+      <c r="GQ1" s="17"/>
+      <c r="GR1" s="17"/>
+      <c r="GS1" s="17"/>
+      <c r="GT1" s="17"/>
+      <c r="GU1" s="17"/>
+      <c r="GV1" s="17"/>
+      <c r="GW1" s="17"/>
+      <c r="GX1" s="17"/>
+      <c r="GY1" s="17"/>
+      <c r="GZ1" s="17"/>
+      <c r="HA1" s="17"/>
+      <c r="HB1" s="17"/>
+      <c r="HC1" s="17"/>
+      <c r="HD1" s="17"/>
+      <c r="HE1" s="17"/>
+      <c r="HF1" s="17"/>
+      <c r="HG1" s="17"/>
+      <c r="HH1" s="17"/>
+      <c r="HI1" s="17"/>
+      <c r="HJ1" s="17"/>
+      <c r="HK1" s="17"/>
+      <c r="HL1" s="17"/>
+      <c r="HM1" s="17"/>
+      <c r="HN1" s="17"/>
+      <c r="HO1" s="17"/>
+      <c r="HP1" s="17"/>
+      <c r="HQ1" s="17"/>
+      <c r="HR1" s="17"/>
+      <c r="HS1" s="17"/>
+      <c r="HT1" s="17"/>
+      <c r="HU1" s="17"/>
+      <c r="HV1" s="17"/>
+      <c r="HW1" s="17"/>
+      <c r="HX1" s="17"/>
+      <c r="HY1" s="17"/>
+      <c r="HZ1" s="17"/>
+      <c r="IA1" s="17"/>
+      <c r="IB1" s="17"/>
+      <c r="IC1" s="17"/>
+      <c r="ID1" s="17"/>
+      <c r="IE1" s="17"/>
+      <c r="IF1" s="17"/>
+      <c r="IG1" s="17"/>
+      <c r="IH1" s="17"/>
+      <c r="II1" s="17"/>
+      <c r="IJ1" s="17"/>
+      <c r="IK1" s="17"/>
+      <c r="IL1" s="17"/>
+      <c r="IM1" s="17"/>
+      <c r="IN1" s="17"/>
+      <c r="IO1" s="17"/>
+      <c r="IP1" s="17"/>
+      <c r="IQ1" s="17"/>
+      <c r="IR1" s="17"/>
+      <c r="IS1" s="17"/>
+      <c r="IT1" s="17"/>
+      <c r="IU1" s="17"/>
+      <c r="IV1" s="17"/>
+      <c r="IW1" s="17"/>
+      <c r="IX1" s="17"/>
+      <c r="IY1" s="17"/>
+      <c r="IZ1" s="17"/>
+      <c r="JA1" s="17"/>
+      <c r="JB1" s="17"/>
+      <c r="JC1" s="17"/>
+      <c r="JD1" s="17"/>
+      <c r="JE1" s="17"/>
+      <c r="JF1" s="17"/>
+      <c r="JG1" s="17"/>
+      <c r="JH1" s="17"/>
+      <c r="JI1" s="17"/>
+      <c r="JJ1" s="17"/>
+      <c r="JK1" s="17"/>
+      <c r="JL1" s="17"/>
+      <c r="JM1" s="17"/>
+      <c r="JN1" s="17"/>
+      <c r="JO1" s="17"/>
+      <c r="JP1" s="17"/>
+      <c r="JQ1" s="17"/>
+      <c r="JR1" s="17"/>
+      <c r="JS1" s="17"/>
+      <c r="JT1" s="17"/>
+      <c r="JU1" s="17"/>
+      <c r="JV1" s="17"/>
+      <c r="JW1" s="17"/>
+      <c r="JX1" s="17"/>
+      <c r="JY1" s="17"/>
+      <c r="JZ1" s="17"/>
+      <c r="KA1" s="17"/>
+      <c r="KB1" s="17"/>
+      <c r="KC1" s="17"/>
+      <c r="KD1" s="17"/>
+      <c r="KE1" s="17"/>
+      <c r="KF1" s="17"/>
+      <c r="KG1" s="17"/>
+      <c r="KH1" s="17"/>
+      <c r="KI1" s="17"/>
+      <c r="KJ1" s="17"/>
+      <c r="KK1" s="17"/>
+      <c r="KL1" s="17"/>
+      <c r="KM1" s="17"/>
+      <c r="KN1" s="17"/>
+      <c r="KO1" s="17"/>
+      <c r="KP1" s="17"/>
+      <c r="KQ1" s="17"/>
+      <c r="KR1" s="17"/>
+      <c r="KS1" s="17"/>
+      <c r="KT1" s="17"/>
+      <c r="KU1" s="17"/>
+      <c r="KV1" s="17"/>
+      <c r="KW1" s="17"/>
+      <c r="KX1" s="17"/>
+      <c r="KY1" s="17"/>
+      <c r="KZ1" s="17"/>
+      <c r="LA1" s="17"/>
+      <c r="LB1" s="17"/>
+      <c r="LC1" s="17"/>
+      <c r="LD1" s="17"/>
+      <c r="LE1" s="17"/>
+      <c r="LF1" s="17"/>
+      <c r="LG1" s="17"/>
+      <c r="LH1" s="17"/>
+      <c r="LI1" s="17"/>
+      <c r="LJ1" s="17"/>
+      <c r="LK1" s="17"/>
+      <c r="LL1" s="17"/>
+      <c r="LM1" s="17"/>
+      <c r="LN1" s="17"/>
+      <c r="LO1" s="17"/>
+      <c r="LP1" s="17"/>
+      <c r="LQ1" s="17"/>
+      <c r="LR1" s="17"/>
+      <c r="LS1" s="17"/>
+      <c r="LT1" s="17"/>
+      <c r="LU1" s="17"/>
+      <c r="LV1" s="17"/>
+      <c r="LW1" s="17"/>
+      <c r="LX1" s="17"/>
+      <c r="LY1" s="17"/>
+      <c r="LZ1" s="17"/>
+      <c r="MA1" s="17"/>
+      <c r="MB1" s="17"/>
+      <c r="MC1" s="17"/>
+      <c r="MD1" s="17"/>
+      <c r="ME1" s="17"/>
+      <c r="MF1" s="17"/>
+      <c r="MG1" s="17"/>
+      <c r="MH1" s="17"/>
+      <c r="MI1" s="17"/>
+      <c r="MJ1" s="17"/>
+      <c r="MK1" s="17"/>
+      <c r="ML1" s="17"/>
+      <c r="MM1" s="17"/>
+      <c r="MN1" s="17"/>
+      <c r="MO1" s="17"/>
+      <c r="MP1" s="17"/>
+      <c r="MQ1" s="17"/>
+      <c r="MR1" s="17"/>
+      <c r="MS1" s="17"/>
+      <c r="MT1" s="17"/>
+      <c r="MU1" s="17"/>
+      <c r="MV1" s="17"/>
+      <c r="MW1" s="17"/>
+      <c r="MX1" s="17"/>
+      <c r="MY1" s="17"/>
+      <c r="MZ1" s="17"/>
+      <c r="NA1" s="17"/>
+      <c r="NB1" s="17"/>
+      <c r="NC1" s="17"/>
+      <c r="ND1" s="17"/>
+      <c r="NE1" s="17"/>
+      <c r="NF1" s="17"/>
+      <c r="NG1" s="17"/>
+      <c r="NH1" s="17"/>
+      <c r="NI1" s="17"/>
+      <c r="NJ1" s="17"/>
+      <c r="NK1" s="17"/>
+      <c r="NL1" s="17"/>
+      <c r="NM1" s="17"/>
+      <c r="NN1" s="17"/>
+      <c r="NO1" s="17"/>
+      <c r="NP1" s="17"/>
+      <c r="NQ1" s="17"/>
+      <c r="NR1" s="17"/>
+      <c r="NS1" s="17"/>
+      <c r="NT1" s="17"/>
+      <c r="NU1" s="17"/>
+      <c r="NV1" s="17"/>
+      <c r="NW1" s="17"/>
+      <c r="NX1" s="17"/>
+      <c r="NY1" s="17"/>
+      <c r="NZ1" s="17"/>
+      <c r="OA1" s="17"/>
+      <c r="OB1" s="17"/>
+      <c r="OC1" s="17"/>
+      <c r="OD1" s="17"/>
+      <c r="OE1" s="17"/>
+      <c r="OF1" s="17"/>
+      <c r="OG1" s="17"/>
+      <c r="OH1" s="17"/>
+      <c r="OI1" s="17"/>
+      <c r="OJ1" s="17"/>
+      <c r="OK1" s="17"/>
+      <c r="OL1" s="17"/>
+      <c r="OM1" s="17"/>
+      <c r="ON1" s="17"/>
+      <c r="OO1" s="17"/>
+      <c r="OP1" s="17"/>
+      <c r="OQ1" s="17"/>
+      <c r="OR1" s="17"/>
+      <c r="OS1" s="17"/>
+      <c r="OT1" s="17"/>
+      <c r="OU1" s="17"/>
+      <c r="OV1" s="17"/>
+      <c r="OW1" s="17"/>
+      <c r="OX1" s="17"/>
+      <c r="OY1" s="17"/>
+      <c r="OZ1" s="17"/>
+      <c r="PA1" s="17"/>
+      <c r="PB1" s="17"/>
+      <c r="PC1" s="17"/>
+      <c r="PD1" s="17"/>
+      <c r="PE1" s="17"/>
+      <c r="PF1" s="17"/>
+      <c r="PG1" s="17"/>
+      <c r="PH1" s="17"/>
+      <c r="PI1" s="17"/>
+      <c r="PJ1" s="17"/>
+      <c r="PK1" s="17"/>
+      <c r="PL1" s="17"/>
+      <c r="PM1" s="17"/>
+      <c r="PN1" s="17"/>
+      <c r="PO1" s="17"/>
+      <c r="PP1" s="17"/>
+      <c r="PQ1" s="17"/>
+      <c r="PR1" s="17"/>
+      <c r="PS1" s="17"/>
+      <c r="PT1" s="17"/>
+      <c r="PU1" s="17"/>
+      <c r="PV1" s="17"/>
+      <c r="PW1" s="17"/>
+      <c r="PX1" s="17"/>
+      <c r="PY1" s="17"/>
+      <c r="PZ1" s="17"/>
+      <c r="QA1" s="17"/>
+      <c r="QB1" s="17"/>
+      <c r="QC1" s="17"/>
+      <c r="QD1" s="17"/>
+      <c r="QE1" s="17"/>
+      <c r="QF1" s="17"/>
+      <c r="QG1" s="17"/>
+      <c r="QH1" s="17"/>
+      <c r="QI1" s="17"/>
+      <c r="QJ1" s="17"/>
+      <c r="QK1" s="17"/>
+      <c r="QL1" s="17"/>
+      <c r="QM1" s="17"/>
+      <c r="QN1" s="17"/>
+      <c r="QO1" s="17"/>
+      <c r="QP1" s="17"/>
+      <c r="QQ1" s="17"/>
+      <c r="QR1" s="17"/>
+      <c r="QS1" s="17"/>
+      <c r="QT1" s="17"/>
+      <c r="QU1" s="17"/>
+      <c r="QV1" s="17"/>
+      <c r="QW1" s="17"/>
+      <c r="QX1" s="17"/>
+      <c r="QY1" s="17"/>
+      <c r="QZ1" s="17"/>
+      <c r="RA1" s="17"/>
+      <c r="RB1" s="17"/>
+      <c r="RC1" s="17"/>
+      <c r="RD1" s="17"/>
+      <c r="RE1" s="17"/>
+      <c r="RF1" s="17"/>
+      <c r="RG1" s="17"/>
+      <c r="RH1" s="17"/>
+      <c r="RI1" s="17"/>
+      <c r="RJ1" s="17"/>
+      <c r="RK1" s="17"/>
+      <c r="RL1" s="17"/>
+      <c r="RM1" s="17"/>
+      <c r="RN1" s="17"/>
+      <c r="RO1" s="17"/>
+      <c r="RP1" s="17"/>
+      <c r="RQ1" s="17"/>
+      <c r="RR1" s="17"/>
+      <c r="RS1" s="17"/>
+      <c r="RT1" s="17"/>
+      <c r="RU1" s="17"/>
+      <c r="RV1" s="17"/>
+      <c r="RW1" s="17"/>
+      <c r="RX1" s="17"/>
+      <c r="RY1" s="17"/>
+      <c r="RZ1" s="17"/>
+      <c r="SA1" s="17"/>
+      <c r="SB1" s="17"/>
+      <c r="SC1" s="17"/>
+      <c r="SD1" s="17"/>
+      <c r="SE1" s="17"/>
+      <c r="SF1" s="17"/>
+      <c r="SG1" s="17"/>
+      <c r="SH1" s="17"/>
+      <c r="SI1" s="17"/>
+      <c r="SJ1" s="17"/>
+      <c r="SK1" s="17"/>
+      <c r="SL1" s="17"/>
+      <c r="SM1" s="17"/>
+      <c r="SN1" s="17"/>
+      <c r="SO1" s="17"/>
+      <c r="SP1" s="17"/>
+      <c r="SQ1" s="17"/>
+      <c r="SR1" s="17"/>
+      <c r="SS1" s="17"/>
+      <c r="ST1" s="17"/>
+      <c r="SU1" s="17"/>
+      <c r="SV1" s="17"/>
+      <c r="SW1" s="17"/>
+      <c r="SX1" s="17"/>
+      <c r="SY1" s="17"/>
+      <c r="SZ1" s="17"/>
+      <c r="TA1" s="17"/>
+      <c r="TB1" s="17"/>
+      <c r="TC1" s="17"/>
+      <c r="TD1" s="17"/>
+      <c r="TE1" s="17"/>
+      <c r="TF1" s="17"/>
+      <c r="TG1" s="17"/>
+      <c r="TH1" s="17"/>
+      <c r="TI1" s="17"/>
+      <c r="TJ1" s="17"/>
+      <c r="TK1" s="17"/>
+      <c r="TL1" s="17"/>
+      <c r="TM1" s="17"/>
+      <c r="TN1" s="17"/>
+      <c r="TO1" s="17"/>
+      <c r="TP1" s="17"/>
+      <c r="TQ1" s="17"/>
+      <c r="TR1" s="17"/>
+      <c r="TS1" s="17"/>
+      <c r="TT1" s="17"/>
+      <c r="TU1" s="17"/>
+      <c r="TV1" s="17"/>
+      <c r="TW1" s="17"/>
+      <c r="TX1" s="17"/>
+      <c r="TY1" s="17"/>
+      <c r="TZ1" s="17"/>
+      <c r="UA1" s="17"/>
+      <c r="UB1" s="17"/>
+      <c r="UC1" s="17"/>
+      <c r="UD1" s="17"/>
+      <c r="UE1" s="17"/>
+      <c r="UF1" s="17"/>
+      <c r="UG1" s="17"/>
+      <c r="UH1" s="17"/>
+      <c r="UI1" s="17"/>
+      <c r="UJ1" s="17"/>
+      <c r="UK1" s="17"/>
+      <c r="UL1" s="17"/>
+      <c r="UM1" s="17"/>
+      <c r="UN1" s="17"/>
+      <c r="UO1" s="17"/>
+      <c r="UP1" s="17"/>
+      <c r="UQ1" s="17"/>
+      <c r="UR1" s="17"/>
+      <c r="US1" s="17"/>
+      <c r="UT1" s="17"/>
+      <c r="UU1" s="17"/>
+      <c r="UV1" s="17"/>
+      <c r="UW1" s="17"/>
+      <c r="UX1" s="17"/>
+      <c r="UY1" s="17"/>
+      <c r="UZ1" s="17"/>
+      <c r="VA1" s="17"/>
+      <c r="VB1" s="17"/>
+      <c r="VC1" s="17"/>
+      <c r="VD1" s="17"/>
+      <c r="VE1" s="17"/>
+      <c r="VF1" s="17"/>
+      <c r="VG1" s="17"/>
+      <c r="VH1" s="17"/>
+      <c r="VI1" s="17"/>
+      <c r="VJ1" s="17"/>
+      <c r="VK1" s="17"/>
+      <c r="VL1" s="17"/>
+      <c r="VM1" s="17"/>
+      <c r="VN1" s="17"/>
+      <c r="VO1" s="17"/>
+      <c r="VP1" s="17"/>
+      <c r="VQ1" s="17"/>
+      <c r="VR1" s="17"/>
+      <c r="VS1" s="17"/>
+      <c r="VT1" s="17"/>
+      <c r="VU1" s="17"/>
+      <c r="VV1" s="17"/>
+      <c r="VW1" s="17"/>
+      <c r="VX1" s="17"/>
+      <c r="VY1" s="17"/>
+      <c r="VZ1" s="17"/>
+      <c r="WA1" s="17"/>
+      <c r="WB1" s="17"/>
+      <c r="WC1" s="17"/>
+      <c r="WD1" s="17"/>
+      <c r="WE1" s="17"/>
+      <c r="WF1" s="17"/>
+      <c r="WG1" s="17"/>
+      <c r="WH1" s="17"/>
+      <c r="WI1" s="17"/>
+      <c r="WJ1" s="17"/>
+      <c r="WK1" s="17"/>
+      <c r="WL1" s="17"/>
+      <c r="WM1" s="17"/>
+      <c r="WN1" s="17"/>
+      <c r="WO1" s="17"/>
+      <c r="WP1" s="17"/>
+      <c r="WQ1" s="17"/>
+      <c r="WR1" s="17"/>
+      <c r="WS1" s="17"/>
+      <c r="WT1" s="17"/>
+      <c r="WU1" s="17"/>
+      <c r="WV1" s="17"/>
+      <c r="WW1" s="17"/>
+      <c r="WX1" s="17"/>
+      <c r="WY1" s="17"/>
+      <c r="WZ1" s="17"/>
+      <c r="XA1" s="17"/>
+      <c r="XB1" s="17"/>
+      <c r="XC1" s="17"/>
+      <c r="XD1" s="17"/>
+      <c r="XE1" s="17"/>
+      <c r="XF1" s="17"/>
+      <c r="XG1" s="17"/>
+      <c r="XH1" s="17"/>
+      <c r="XI1" s="17"/>
+      <c r="XJ1" s="17"/>
+      <c r="XK1" s="17"/>
+      <c r="XL1" s="17"/>
+      <c r="XM1" s="17"/>
+      <c r="XN1" s="17"/>
+      <c r="XO1" s="17"/>
+      <c r="XP1" s="17"/>
+      <c r="XQ1" s="17"/>
+      <c r="XR1" s="17"/>
+      <c r="XS1" s="17"/>
+      <c r="XT1" s="17"/>
+      <c r="XU1" s="17"/>
+      <c r="XV1" s="17"/>
+      <c r="XW1" s="17"/>
+      <c r="XX1" s="17"/>
+      <c r="XY1" s="17"/>
+      <c r="XZ1" s="17"/>
+      <c r="YA1" s="17"/>
+      <c r="YB1" s="17"/>
+      <c r="YC1" s="17"/>
+      <c r="YD1" s="17"/>
+      <c r="YE1" s="17"/>
+      <c r="YF1" s="17"/>
+      <c r="YG1" s="17"/>
+      <c r="YH1" s="17"/>
+      <c r="YI1" s="17"/>
+      <c r="YJ1" s="17"/>
+      <c r="YK1" s="17"/>
+      <c r="YL1" s="17"/>
+      <c r="YM1" s="17"/>
+      <c r="YN1" s="17"/>
+      <c r="YO1" s="17"/>
+      <c r="YP1" s="17"/>
+      <c r="YQ1" s="17"/>
+      <c r="YR1" s="17"/>
+      <c r="YS1" s="17"/>
+      <c r="YT1" s="17"/>
+      <c r="YU1" s="17"/>
+      <c r="YV1" s="17"/>
+      <c r="YW1" s="17"/>
+      <c r="YX1" s="17"/>
+      <c r="YY1" s="17"/>
+      <c r="YZ1" s="17"/>
+      <c r="ZA1" s="17"/>
+      <c r="ZB1" s="17"/>
+      <c r="ZC1" s="17"/>
+      <c r="ZD1" s="17"/>
+      <c r="ZE1" s="17"/>
+      <c r="ZF1" s="17"/>
+      <c r="ZG1" s="17"/>
+      <c r="ZH1" s="17"/>
+      <c r="ZI1" s="17"/>
+      <c r="ZJ1" s="17"/>
+      <c r="ZK1" s="17"/>
+      <c r="ZL1" s="17"/>
+      <c r="ZM1" s="17"/>
+      <c r="ZN1" s="17"/>
+      <c r="ZO1" s="17"/>
+      <c r="ZP1" s="17"/>
+      <c r="ZQ1" s="17"/>
+      <c r="ZR1" s="17"/>
+      <c r="ZS1" s="17"/>
+      <c r="ZT1" s="17"/>
+      <c r="ZU1" s="17"/>
+      <c r="ZV1" s="17"/>
+      <c r="ZW1" s="17"/>
+      <c r="ZX1" s="17"/>
+      <c r="ZY1" s="17"/>
+      <c r="ZZ1" s="17"/>
+      <c r="AAA1" s="17"/>
+      <c r="AAB1" s="17"/>
+      <c r="AAC1" s="17"/>
+      <c r="AAD1" s="17"/>
+      <c r="AAE1" s="17"/>
+      <c r="AAF1" s="17"/>
+      <c r="AAG1" s="17"/>
+      <c r="AAH1" s="17"/>
+      <c r="AAI1" s="17"/>
+      <c r="AAJ1" s="17"/>
+      <c r="AAK1" s="17"/>
+      <c r="AAL1" s="17"/>
+      <c r="AAM1" s="17"/>
+      <c r="AAN1" s="17"/>
+      <c r="AAO1" s="17"/>
+      <c r="AAP1" s="17"/>
+      <c r="AAQ1" s="17"/>
+      <c r="AAR1" s="17"/>
+      <c r="AAS1" s="17"/>
+      <c r="AAT1" s="17"/>
+      <c r="AAU1" s="17"/>
+      <c r="AAV1" s="17"/>
+      <c r="AAW1" s="17"/>
+      <c r="AAX1" s="17"/>
+      <c r="AAY1" s="17"/>
+      <c r="AAZ1" s="17"/>
+      <c r="ABA1" s="17"/>
+      <c r="ABB1" s="17"/>
+      <c r="ABC1" s="17"/>
+      <c r="ABD1" s="17"/>
+      <c r="ABE1" s="17"/>
+      <c r="ABF1" s="17"/>
+      <c r="ABG1" s="17"/>
+      <c r="ABH1" s="17"/>
+      <c r="ABI1" s="17"/>
+      <c r="ABJ1" s="17"/>
+      <c r="ABK1" s="17"/>
+      <c r="ABL1" s="17"/>
+      <c r="ABM1" s="17"/>
+      <c r="ABN1" s="17"/>
+      <c r="ABO1" s="17"/>
+      <c r="ABP1" s="17"/>
+      <c r="ABQ1" s="17"/>
+      <c r="ABR1" s="17"/>
+      <c r="ABS1" s="17"/>
+      <c r="ABT1" s="17"/>
+      <c r="ABU1" s="17"/>
+      <c r="ABV1" s="17"/>
+      <c r="ABW1" s="17"/>
+      <c r="ABX1" s="17"/>
+      <c r="ABY1" s="17"/>
+      <c r="ABZ1" s="17"/>
+      <c r="ACA1" s="17"/>
+      <c r="ACB1" s="17"/>
+      <c r="ACC1" s="17"/>
+      <c r="ACD1" s="17"/>
+      <c r="ACE1" s="17"/>
+      <c r="ACF1" s="17"/>
+      <c r="ACG1" s="17"/>
+      <c r="ACH1" s="17"/>
+      <c r="ACI1" s="17"/>
+      <c r="ACJ1" s="17"/>
+      <c r="ACK1" s="17"/>
+      <c r="ACL1" s="17"/>
+      <c r="ACM1" s="17"/>
+      <c r="ACN1" s="17"/>
+      <c r="ACO1" s="17"/>
+      <c r="ACP1" s="17"/>
+      <c r="ACQ1" s="17"/>
+      <c r="ACR1" s="17"/>
+      <c r="ACS1" s="17"/>
+      <c r="ACT1" s="17"/>
+      <c r="ACU1" s="17"/>
+      <c r="ACV1" s="17"/>
+      <c r="ACW1" s="17"/>
+      <c r="ACX1" s="17"/>
+      <c r="ACY1" s="17"/>
+      <c r="ACZ1" s="17"/>
+      <c r="ADA1" s="17"/>
+      <c r="ADB1" s="17"/>
+      <c r="ADC1" s="17"/>
+      <c r="ADD1" s="17"/>
+      <c r="ADE1" s="17"/>
+      <c r="ADF1" s="17"/>
+      <c r="ADG1" s="17"/>
+      <c r="ADH1" s="17"/>
+      <c r="ADI1" s="17"/>
+      <c r="ADJ1" s="17"/>
+      <c r="ADK1" s="17"/>
+      <c r="ADL1" s="17"/>
+      <c r="ADM1" s="17"/>
+      <c r="ADN1" s="17"/>
+      <c r="ADO1" s="17"/>
+      <c r="ADP1" s="17"/>
+      <c r="ADQ1" s="17"/>
+      <c r="ADR1" s="17"/>
+      <c r="ADS1" s="17"/>
+      <c r="ADT1" s="17"/>
+      <c r="ADU1" s="17"/>
+      <c r="ADV1" s="17"/>
+      <c r="ADW1" s="17"/>
+      <c r="ADX1" s="17"/>
+      <c r="ADY1" s="17"/>
+      <c r="ADZ1" s="17"/>
+      <c r="AEA1" s="17"/>
+      <c r="AEB1" s="17"/>
+      <c r="AEC1" s="17"/>
+      <c r="AED1" s="17"/>
+      <c r="AEE1" s="17"/>
+      <c r="AEF1" s="17"/>
+      <c r="AEG1" s="17"/>
+      <c r="AEH1" s="17"/>
+      <c r="AEI1" s="17"/>
+      <c r="AEJ1" s="17"/>
+      <c r="AEK1" s="17"/>
+      <c r="AEL1" s="17"/>
+      <c r="AEM1" s="17"/>
+      <c r="AEN1" s="17"/>
+      <c r="AEO1" s="17"/>
+      <c r="AEP1" s="17"/>
+      <c r="AEQ1" s="17"/>
+      <c r="AER1" s="17"/>
+      <c r="AES1" s="17"/>
+      <c r="AET1" s="17"/>
+      <c r="AEU1" s="17"/>
+      <c r="AEV1" s="17"/>
+      <c r="AEW1" s="17"/>
+      <c r="AEX1" s="17"/>
+      <c r="AEY1" s="17"/>
+      <c r="AEZ1" s="17"/>
+      <c r="AFA1" s="17"/>
+      <c r="AFB1" s="17"/>
+      <c r="AFC1" s="17"/>
+      <c r="AFD1" s="17"/>
+      <c r="AFE1" s="17"/>
+      <c r="AFF1" s="17"/>
+      <c r="AFG1" s="17"/>
+      <c r="AFH1" s="17"/>
+      <c r="AFI1" s="17"/>
+      <c r="AFJ1" s="17"/>
+      <c r="AFK1" s="17"/>
+      <c r="AFL1" s="17"/>
+      <c r="AFM1" s="17"/>
+      <c r="AFN1" s="17"/>
+      <c r="AFO1" s="17"/>
+      <c r="AFP1" s="17"/>
+      <c r="AFQ1" s="17"/>
+      <c r="AFR1" s="17"/>
+      <c r="AFS1" s="17"/>
+      <c r="AFT1" s="17"/>
+      <c r="AFU1" s="17"/>
+      <c r="AFV1" s="17"/>
+      <c r="AFW1" s="17"/>
+      <c r="AFX1" s="17"/>
+      <c r="AFY1" s="17"/>
+      <c r="AFZ1" s="17"/>
+      <c r="AGA1" s="17"/>
+      <c r="AGB1" s="17"/>
+      <c r="AGC1" s="17"/>
+      <c r="AGD1" s="17"/>
+      <c r="AGE1" s="17"/>
+      <c r="AGF1" s="17"/>
+      <c r="AGG1" s="17"/>
+      <c r="AGH1" s="17"/>
+      <c r="AGI1" s="17"/>
+      <c r="AGJ1" s="17"/>
+      <c r="AGK1" s="17"/>
+      <c r="AGL1" s="17"/>
+      <c r="AGM1" s="17"/>
+      <c r="AGN1" s="17"/>
+      <c r="AGO1" s="17"/>
+      <c r="AGP1" s="17"/>
+      <c r="AGQ1" s="17"/>
+      <c r="AGR1" s="17"/>
+      <c r="AGS1" s="17"/>
+      <c r="AGT1" s="17"/>
+      <c r="AGU1" s="17"/>
+      <c r="AGV1" s="17"/>
+      <c r="AGW1" s="17"/>
+      <c r="AGX1" s="17"/>
+      <c r="AGY1" s="17"/>
+      <c r="AGZ1" s="17"/>
+      <c r="AHA1" s="17"/>
+      <c r="AHB1" s="17"/>
+      <c r="AHC1" s="17"/>
+      <c r="AHD1" s="17"/>
+      <c r="AHE1" s="17"/>
+      <c r="AHF1" s="17"/>
+      <c r="AHG1" s="17"/>
+      <c r="AHH1" s="17"/>
+      <c r="AHI1" s="17"/>
+      <c r="AHJ1" s="17"/>
+      <c r="AHK1" s="17"/>
+      <c r="AHL1" s="17"/>
+      <c r="AHM1" s="17"/>
+      <c r="AHN1" s="17"/>
+      <c r="AHO1" s="17"/>
+      <c r="AHP1" s="17"/>
+      <c r="AHQ1" s="17"/>
+      <c r="AHR1" s="17"/>
+      <c r="AHS1" s="17"/>
+      <c r="AHT1" s="17"/>
+      <c r="AHU1" s="17"/>
+      <c r="AHV1" s="17"/>
+      <c r="AHW1" s="17"/>
+      <c r="AHX1" s="17"/>
+      <c r="AHY1" s="17"/>
+      <c r="AHZ1" s="17"/>
+      <c r="AIA1" s="17"/>
+      <c r="AIB1" s="17"/>
+      <c r="AIC1" s="17"/>
+      <c r="AID1" s="17"/>
+      <c r="AIE1" s="17"/>
+      <c r="AIF1" s="17"/>
+      <c r="AIG1" s="17"/>
+      <c r="AIH1" s="17"/>
+      <c r="AII1" s="17"/>
+      <c r="AIJ1" s="17"/>
+      <c r="AIK1" s="17"/>
+      <c r="AIL1" s="17"/>
+      <c r="AIM1" s="17"/>
+      <c r="AIN1" s="17"/>
+      <c r="AIO1" s="17"/>
+      <c r="AIP1" s="17"/>
+      <c r="AIQ1" s="17"/>
+      <c r="AIR1" s="17"/>
+      <c r="AIS1" s="17"/>
+      <c r="AIT1" s="17"/>
+      <c r="AIU1" s="17"/>
+      <c r="AIV1" s="17"/>
+      <c r="AIW1" s="17"/>
+      <c r="AIX1" s="17"/>
+      <c r="AIY1" s="17"/>
+      <c r="AIZ1" s="17"/>
+      <c r="AJA1" s="17"/>
+      <c r="AJB1" s="17"/>
+      <c r="AJC1" s="17"/>
+      <c r="AJD1" s="17"/>
+      <c r="AJE1" s="17"/>
+      <c r="AJF1" s="17"/>
+      <c r="AJG1" s="17"/>
+      <c r="AJH1" s="17"/>
+      <c r="AJI1" s="17"/>
+      <c r="AJJ1" s="17"/>
+      <c r="AJK1" s="17"/>
+      <c r="AJL1" s="17"/>
+      <c r="AJM1" s="17"/>
+      <c r="AJN1" s="17"/>
+      <c r="AJO1" s="17"/>
+      <c r="AJP1" s="17"/>
+      <c r="AJQ1" s="17"/>
+      <c r="AJR1" s="17"/>
+      <c r="AJS1" s="17"/>
+      <c r="AJT1" s="17"/>
+      <c r="AJU1" s="17"/>
+      <c r="AJV1" s="17"/>
+      <c r="AJW1" s="17"/>
+      <c r="AJX1" s="17"/>
+      <c r="AJY1" s="17"/>
+      <c r="AJZ1" s="17"/>
+      <c r="AKA1" s="17"/>
+      <c r="AKB1" s="17"/>
+      <c r="AKC1" s="17"/>
+      <c r="AKD1" s="17"/>
+      <c r="AKE1" s="17"/>
+      <c r="AKF1" s="17"/>
+      <c r="AKG1" s="17"/>
+      <c r="AKH1" s="17"/>
+      <c r="AKI1" s="17"/>
+      <c r="AKJ1" s="17"/>
+      <c r="AKK1" s="17"/>
+      <c r="AKL1" s="17"/>
+      <c r="AKM1" s="17"/>
+      <c r="AKN1" s="17"/>
+      <c r="AKO1" s="17"/>
+      <c r="AKP1" s="17"/>
+      <c r="AKQ1" s="17"/>
+      <c r="AKR1" s="17"/>
+      <c r="AKS1" s="17"/>
+      <c r="AKT1" s="17"/>
+      <c r="AKU1" s="17"/>
+      <c r="AKV1" s="17"/>
+      <c r="AKW1" s="17"/>
+      <c r="AKX1" s="17"/>
+      <c r="AKY1" s="17"/>
+      <c r="AKZ1" s="17"/>
+      <c r="ALA1" s="17"/>
+      <c r="ALB1" s="17"/>
+      <c r="ALC1" s="17"/>
+      <c r="ALD1" s="17"/>
+      <c r="ALE1" s="17"/>
+      <c r="ALF1" s="17"/>
+      <c r="ALG1" s="17"/>
+      <c r="ALH1" s="17"/>
+      <c r="ALI1" s="17"/>
+      <c r="ALJ1" s="17"/>
+      <c r="ALK1" s="17"/>
+      <c r="ALL1" s="17"/>
+      <c r="ALM1" s="17"/>
+      <c r="ALN1" s="17"/>
+      <c r="ALO1" s="17"/>
+      <c r="ALP1" s="17"/>
+      <c r="ALQ1" s="17"/>
+      <c r="ALR1" s="17"/>
+      <c r="ALS1" s="17"/>
+      <c r="ALT1" s="17"/>
+      <c r="ALU1" s="17"/>
+      <c r="ALV1" s="17"/>
+      <c r="ALW1" s="17"/>
+      <c r="ALX1" s="17"/>
+      <c r="ALY1" s="17"/>
+      <c r="ALZ1" s="17"/>
+      <c r="AMA1" s="17"/>
+      <c r="AMB1" s="17"/>
+      <c r="AMC1" s="17"/>
+      <c r="AMD1" s="17"/>
+      <c r="AME1" s="17"/>
+      <c r="AMF1" s="17"/>
+      <c r="AMG1" s="17"/>
+      <c r="AMH1" s="17"/>
+      <c r="AMI1" s="17"/>
+      <c r="AMJ1" s="17"/>
+      <c r="AMK1" s="17"/>
+      <c r="AML1" s="17"/>
+      <c r="AMM1" s="17"/>
+      <c r="AMN1" s="17"/>
+      <c r="AMO1" s="17"/>
+      <c r="AMP1" s="17"/>
+      <c r="AMQ1" s="17"/>
+      <c r="AMR1" s="17"/>
       <c r="AMS1"/>
       <c r="AMT1"/>
       <c r="AMU1"/>
@@ -20498,8 +20479,8 @@
       <c r="XFC1"/>
       <c r="XFD1"/>
     </row>
-    <row r="2" s="18" customFormat="1" ht="15.1" customHeight="1" spans="1:16384">
-      <c r="A2" s="27" t="s">
+    <row r="2" s="17" customFormat="1" ht="15.1" customHeight="1" spans="1:16384">
+      <c r="A2" s="26" t="s">
         <v>25</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -20536,28 +20517,32 @@
         <v>72</v>
       </c>
       <c r="M2" s="2" t="s">
-        <v>73</v>
+        <v>68</v>
       </c>
       <c r="N2" s="2" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="2" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="2" t="s">
         <v>71</v>
       </c>
-      <c r="O2" s="2" t="s">
+      <c r="Q2" s="2" t="s">
         <v>40</v>
       </c>
-      <c r="P2" s="2" t="s">
+      <c r="R2" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="Q2" s="2" t="s">
+      <c r="S2" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="R2" s="2" t="s">
+      <c r="T2" s="2" t="s">
         <v>41</v>
       </c>
-      <c r="S2" s="2" t="s">
+      <c r="U2" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AMQ2"/>
-      <c r="AMR2"/>
       <c r="AMS2"/>
       <c r="AMT2"/>
       <c r="AMU2"/>
@@ -35911,30 +35896,30 @@
       <c r="XFC2"/>
       <c r="XFD2"/>
     </row>
-    <row r="3" customHeight="1" spans="1:18">
-      <c r="A3" s="17" t="s">
+    <row r="3" customHeight="1" spans="1:20">
+      <c r="A3" s="16" t="s">
+        <v>73</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>74</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="1" t="s">
         <v>75</v>
       </c>
-      <c r="C3" s="1" t="s">
+      <c r="D3" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="1" t="s">
+      <c r="E3" s="1" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="1" t="s">
+      <c r="F3" s="1" t="s">
         <v>78</v>
       </c>
-      <c r="F3" s="1" t="s">
+      <c r="G3" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G3" s="1" t="s">
+      <c r="H3" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="H3" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="I3" s="9">
         <v>4.58e-17</v>
@@ -35943,43 +35928,49 @@
         <v>4.58e-18</v>
       </c>
       <c r="K3" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="L3" s="1" t="s">
         <v>82</v>
       </c>
-      <c r="L3" s="1" t="s">
+      <c r="M3" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N3" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="O3" s="1">
+        <v>0.775</v>
+      </c>
+      <c r="P3" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="M3" s="1">
-        <v>7.75</v>
-      </c>
-      <c r="N3" s="1" t="s">
+      <c r="T3" s="16" t="s">
         <v>84</v>
       </c>
-      <c r="R3" s="17" t="s">
+    </row>
+    <row r="4" customHeight="1" spans="1:20">
+      <c r="A4" s="16" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="4" customHeight="1" spans="1:18">
-      <c r="A4" s="17" t="s">
-        <v>79</v>
-      </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="1" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="1" t="s">
-        <v>87</v>
-      </c>
       <c r="D4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="E4" s="1" t="s">
         <v>77</v>
-      </c>
-      <c r="E4" s="1" t="s">
-        <v>78</v>
       </c>
       <c r="F4" s="1"/>
       <c r="G4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H4" s="1" t="s">
         <v>80</v>
-      </c>
-      <c r="H4" s="1" t="s">
-        <v>81</v>
       </c>
       <c r="I4" s="9">
         <v>1e-12</v>
@@ -35988,19 +35979,25 @@
         <v>1e-13</v>
       </c>
       <c r="K4" s="1" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="L4" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="N4" s="1">
+        <v>7.75</v>
+      </c>
+      <c r="O4" s="1">
+        <v>0.775</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="T4" s="16" t="s">
         <v>88</v>
-      </c>
-      <c r="M4" s="1">
-        <v>7.75</v>
-      </c>
-      <c r="N4" s="1" t="s">
-        <v>84</v>
-      </c>
-      <c r="R4" s="17" t="s">
-        <v>89</v>
       </c>
     </row>
   </sheetData>
@@ -36009,7 +36006,7 @@
   </autoFilter>
   <mergeCells count="2">
     <mergeCell ref="H1:K1"/>
-    <mergeCell ref="M1:N1"/>
+    <mergeCell ref="M1:P1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="1" firstPageNumber="0" orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
@@ -36032,14 +36029,14 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="3" width="8.78333333333333" style="17"/>
-    <col min="4" max="4" width="16.125" style="17" customWidth="1"/>
-    <col min="5" max="10" width="8.78333333333333" style="17"/>
-    <col min="11" max="1026" width="8.78333333333333" style="25"/>
-    <col min="1027" max="16384" width="9" style="25"/>
+    <col min="1" max="3" width="8.78333333333333" style="16"/>
+    <col min="4" max="4" width="16.125" style="16" customWidth="1"/>
+    <col min="5" max="10" width="8.78333333333333" style="16"/>
+    <col min="11" max="1026" width="8.78333333333333" style="24"/>
+    <col min="1027" max="16384" width="9" style="24"/>
   </cols>
   <sheetData>
-    <row r="1" s="18" customFormat="1" customHeight="1" spans="1:1025">
+    <row r="1" s="17" customFormat="1" customHeight="1" spans="1:1025">
       <c r="A1" s="2" t="s">
         <v>25</v>
       </c>
@@ -36047,19 +36044,19 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>93</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>94</v>
       </c>
       <c r="H1" s="2" t="s">
         <v>40</v>
@@ -36076,136 +36073,136 @@
       <c r="L1" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="AMK1" s="25"/>
+      <c r="AMK1" s="24"/>
     </row>
     <row r="2" customHeight="1" spans="1:8">
-      <c r="A2" s="17" t="s">
+      <c r="A2" s="16" t="s">
+        <v>94</v>
+      </c>
+      <c r="B2" s="16" t="s">
         <v>95</v>
       </c>
-      <c r="B2" s="17" t="s">
+      <c r="C2" s="24"/>
+      <c r="D2" s="16" t="s">
         <v>96</v>
       </c>
-      <c r="C2" s="25"/>
-      <c r="D2" s="17" t="s">
+      <c r="E2" s="16">
+        <v>1</v>
+      </c>
+      <c r="F2" s="16">
+        <v>0</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>97</v>
       </c>
-      <c r="E2" s="17">
-        <v>1</v>
-      </c>
-      <c r="F2" s="17">
-        <v>0</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H2" s="26"/>
+      <c r="H2" s="25"/>
     </row>
     <row r="3" customHeight="1" spans="1:8">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="16" t="s">
+        <v>98</v>
+      </c>
+      <c r="B3" s="16" t="s">
         <v>99</v>
       </c>
-      <c r="B3" s="17" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="C3" s="25"/>
-      <c r="D3" s="17" t="s">
-        <v>101</v>
-      </c>
-      <c r="E3" s="17">
+      <c r="E3" s="16">
         <v>2</v>
       </c>
-      <c r="F3" s="17">
+      <c r="F3" s="16">
         <v>0</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H3" s="26"/>
+        <v>97</v>
+      </c>
+      <c r="H3" s="25"/>
     </row>
     <row r="4" customHeight="1" spans="1:8">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
+        <v>101</v>
+      </c>
+      <c r="B4" s="16" t="s">
         <v>102</v>
       </c>
-      <c r="B4" s="17" t="s">
+      <c r="C4" s="24"/>
+      <c r="D4" s="16" t="s">
         <v>103</v>
       </c>
-      <c r="C4" s="25"/>
-      <c r="D4" s="17" t="s">
-        <v>104</v>
-      </c>
-      <c r="E4" s="17">
+      <c r="E4" s="16">
         <v>3</v>
       </c>
-      <c r="F4" s="17">
+      <c r="F4" s="16">
         <v>0</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H4" s="26"/>
+        <v>97</v>
+      </c>
+      <c r="H4" s="25"/>
     </row>
     <row r="5" customHeight="1" spans="1:8">
-      <c r="A5" s="25" t="s">
+      <c r="A5" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="24" t="s">
         <v>105</v>
       </c>
-      <c r="B5" s="25" t="s">
+      <c r="C5" s="24"/>
+      <c r="D5" s="16" t="s">
         <v>106</v>
       </c>
-      <c r="C5" s="25"/>
-      <c r="D5" s="17" t="s">
-        <v>107</v>
-      </c>
-      <c r="E5" s="25">
+      <c r="E5" s="24">
         <v>4</v>
       </c>
-      <c r="F5" s="17">
+      <c r="F5" s="16">
         <v>0</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H5" s="26"/>
+        <v>97</v>
+      </c>
+      <c r="H5" s="25"/>
     </row>
     <row r="6" customHeight="1" spans="1:8">
-      <c r="A6" s="25" t="s">
+      <c r="A6" s="24" t="s">
+        <v>107</v>
+      </c>
+      <c r="B6" s="24" t="s">
         <v>108</v>
       </c>
-      <c r="B6" s="25" t="s">
+      <c r="C6" s="24"/>
+      <c r="D6" s="16" t="s">
         <v>109</v>
       </c>
-      <c r="C6" s="25"/>
-      <c r="D6" s="17" t="s">
-        <v>110</v>
-      </c>
-      <c r="E6" s="25">
+      <c r="E6" s="24">
         <v>5</v>
       </c>
-      <c r="F6" s="17">
+      <c r="F6" s="16">
         <v>0</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="H6" s="26"/>
+        <v>97</v>
+      </c>
+      <c r="H6" s="25"/>
     </row>
     <row r="7" customHeight="1" spans="1:7">
-      <c r="A7" s="25" t="s">
+      <c r="A7" s="24" t="s">
+        <v>110</v>
+      </c>
+      <c r="B7" s="24" t="s">
         <v>111</v>
       </c>
-      <c r="B7" s="25" t="s">
+      <c r="D7" s="16" t="s">
         <v>112</v>
       </c>
-      <c r="D7" s="17" t="s">
-        <v>113</v>
-      </c>
-      <c r="E7" s="25">
+      <c r="E7" s="24">
         <v>6</v>
       </c>
-      <c r="F7" s="17">
+      <c r="F7" s="16">
         <v>0</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="8:8">
@@ -36218,7 +36215,7 @@
       <c r="H11" s="1"/>
     </row>
     <row r="12" customHeight="1" spans="8:8">
-      <c r="H12" s="19"/>
+      <c r="H12" s="18"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:I7">
@@ -36258,10 +36255,10 @@
         <v>27</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>113</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>114</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>115</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>71</v>
@@ -36284,114 +36281,114 @@
     </row>
     <row r="2" customHeight="1" spans="1:5">
       <c r="A2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="E2" s="1" t="s">
         <v>116</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>95</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:5">
       <c r="A3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:5">
       <c r="A4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:5">
       <c r="A5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:5">
       <c r="A6" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:5">
       <c r="A7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="8" customHeight="1" spans="1:5">
       <c r="A8" s="1" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D8" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="9" customHeight="1" spans="1:5">
       <c r="A9" s="1" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="D9" s="1" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
   </sheetData>
@@ -36468,104 +36465,104 @@
     </row>
     <row r="2" customHeight="1" spans="1:7">
       <c r="A2" s="1" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="E2" s="23">
+        <v>0.000148</v>
+      </c>
+      <c r="G2" s="23" t="s">
         <v>125</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>116</v>
-      </c>
-      <c r="D2" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E2" s="24">
-        <v>0.000148</v>
-      </c>
-      <c r="G2" s="24" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="3" customHeight="1" spans="1:7">
       <c r="A3" s="1" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E3" s="24">
+        <v>80</v>
+      </c>
+      <c r="E3" s="23">
         <v>0.0002</v>
       </c>
-      <c r="G3" s="24" t="s">
-        <v>126</v>
+      <c r="G3" s="23" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="4" customHeight="1" spans="1:7">
       <c r="A4" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E4" s="24">
+        <v>80</v>
+      </c>
+      <c r="E4" s="23">
         <v>0.0005</v>
       </c>
-      <c r="G4" s="24" t="s">
-        <v>126</v>
+      <c r="G4" s="23" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="5" customHeight="1" spans="1:7">
       <c r="A5" s="1" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E5" s="24">
+        <v>80</v>
+      </c>
+      <c r="E5" s="23">
         <v>0.0005</v>
       </c>
-      <c r="G5" s="24" t="s">
-        <v>126</v>
+      <c r="G5" s="23" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="6" customHeight="1" spans="1:7">
       <c r="A6" s="1" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E6" s="24">
+        <v>80</v>
+      </c>
+      <c r="E6" s="23">
         <v>0.001</v>
       </c>
-      <c r="G6" s="24" t="s">
-        <v>126</v>
+      <c r="G6" s="23" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="7" customHeight="1" spans="1:7">
       <c r="A7" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>81</v>
-      </c>
-      <c r="E7" s="24">
+        <v>80</v>
+      </c>
+      <c r="E7" s="23">
         <v>0.002</v>
       </c>
-      <c r="G7" s="24" t="s">
-        <v>126</v>
+      <c r="G7" s="23" t="s">
+        <v>125</v>
       </c>
     </row>
   </sheetData>

</xml_diff>